<commit_message>
Made all spreadsheets the demo so that it's not broken, until new spreadsheets are merged in
</commit_message>
<xml_diff>
--- a/applications/demo/data/regional/demoregion1_input.xlsx
+++ b/applications/demo/data/regional/demoregion1_input.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10523"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/demo/data/national/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0064327A-C7AE-F14C-953C-BBBAFF95EA77}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-21135" windowWidth="28920" windowHeight="16320" tabRatio="961" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="961" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -21,12 +27,18 @@
     <sheet name="Reference programs" sheetId="59" state="hidden" r:id="rId12"/>
     <sheet name="Incidence of conditions" sheetId="7" r:id="rId13"/>
     <sheet name="Programs target population" sheetId="21" r:id="rId14"/>
-    <sheet name="Programs family planning" sheetId="54" state="hidden" r:id="rId15"/>
+    <sheet name="Cost curve options" sheetId="61" state="hidden" r:id="rId15"/>
+    <sheet name="Programs family planning" sheetId="54" state="hidden" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="abortion" localSheetId="6">'Baseline year population inputs'!$C$37</definedName>
     <definedName name="abortion">'Baseline year population inputs'!$C$40</definedName>
     <definedName name="comm_deliv">'Treatment of SAM'!$D$3</definedName>
+    <definedName name="diarrhoea_1_5mo">'Baseline year population inputs'!$C$51</definedName>
+    <definedName name="diarrhoea_12_23mo">'Baseline year population inputs'!$C$53</definedName>
+    <definedName name="diarrhoea_1mo">'Baseline year population inputs'!$C$50</definedName>
+    <definedName name="diarrhoea_24_59mo">'Baseline year population inputs'!$C$54</definedName>
+    <definedName name="diarrhoea_6_11mo">'Baseline year population inputs'!$C$52</definedName>
     <definedName name="end_year">'Baseline year population inputs'!$C$4</definedName>
     <definedName name="famplan_unmet_need">'Baseline year population inputs'!$C$12</definedName>
     <definedName name="food_insecure">'Baseline year population inputs'!$C$7</definedName>
@@ -67,7 +79,7 @@
     <definedName name="term_SGA">'Baseline year population inputs'!$C$46</definedName>
     <definedName name="U5_mortality">'Baseline year population inputs'!$C$38</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -77,12 +89,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -106,7 +118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000002000000}">
       <text>
         <r>
           <rPr>
@@ -135,12 +147,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0E00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -178,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="210">
   <si>
     <t>year</t>
   </si>
@@ -771,9 +783,6 @@
     <t>Baseline year (projection start year)</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>Unit costs (US$) by delivery modality and target population</t>
   </si>
   <si>
@@ -796,19 +805,34 @@
   </si>
   <si>
     <t>Unit cost (US$)</t>
+  </si>
+  <si>
+    <t>Decreasing</t>
+  </si>
+  <si>
+    <t>Increasing</t>
+  </si>
+  <si>
+    <t>Mixed</t>
+  </si>
+  <si>
+    <t>Constant (default)</t>
+  </si>
+  <si>
+    <t>Marginal cost to coverage relationship</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -936,12 +960,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="0" tint="-4.9989318521683403E-2"/>
       <name val="Arial"/>
@@ -1784,7 +1802,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1919,8 +1937,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="725" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="725" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="725" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1935,9 +1951,6 @@
     <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="9" fillId="3" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="725" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="725" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="725" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1951,13 +1964,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="726" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="21" fillId="3" borderId="4" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="725" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1966,6 +1978,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="4" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="725" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="727">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
@@ -2692,8 +2711,8 @@
     <cellStyle name="Hyperlink" xfId="721" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="723" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="725"/>
-    <cellStyle name="Normal 3" xfId="726"/>
+    <cellStyle name="Normal 2" xfId="725" xr:uid="{00000000-0005-0000-0000-0000D4020000}"/>
+    <cellStyle name="Normal 3" xfId="726" xr:uid="{00000000-0005-0000-0000-0000D5020000}"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
   <dxfs count="1">
@@ -2752,7 +2771,7 @@
         <xdr:cNvPr id="2049" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000001080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000001080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2809,7 +2828,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2866,7 +2885,7 @@
         <xdr:cNvPr id="3" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2923,7 +2942,7 @@
         <xdr:cNvPr id="4" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2980,7 +2999,7 @@
         <xdr:cNvPr id="5" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3037,7 +3056,7 @@
         <xdr:cNvPr id="6" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3094,7 +3113,7 @@
         <xdr:cNvPr id="7" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3151,7 +3170,7 @@
         <xdr:cNvPr id="8" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3208,7 +3227,7 @@
         <xdr:cNvPr id="9" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3265,7 +3284,7 @@
         <xdr:cNvPr id="10" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3322,7 +3341,7 @@
         <xdr:cNvPr id="11" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3379,7 +3398,7 @@
         <xdr:cNvPr id="12" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3436,7 +3455,7 @@
         <xdr:cNvPr id="13" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3493,7 +3512,7 @@
         <xdr:cNvPr id="14" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3550,7 +3569,7 @@
         <xdr:cNvPr id="15" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3607,7 +3626,7 @@
         <xdr:cNvPr id="16" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000010000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3664,7 +3683,7 @@
         <xdr:cNvPr id="17" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000011000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3721,7 +3740,7 @@
         <xdr:cNvPr id="18" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000012000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3770,7 +3789,7 @@
         <xdr:cNvPr id="19" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000013000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4133,24 +4152,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" style="15" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" style="19" customWidth="1"/>
-    <col min="3" max="16384" width="14.42578125" style="15"/>
+    <col min="1" max="1" width="27.6640625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" style="19" customWidth="1"/>
+    <col min="3" max="16384" width="14.5" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>100</v>
       </c>
@@ -4161,42 +4180,42 @@
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="15" t="s">
         <v>194</v>
       </c>
       <c r="B2" s="59"/>
       <c r="C2" s="59"/>
     </row>
-    <row r="3" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="C3" s="92">
+      <c r="C3" s="86">
         <v>2017</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="C4" s="93">
+      <c r="C4" s="87">
         <v>2030</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
     </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="9" t="s">
         <v>106</v>
       </c>
@@ -4204,7 +4223,7 @@
         <v>0.28199999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="12" t="s">
         <v>107</v>
       </c>
@@ -4212,7 +4231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="12" t="s">
         <v>105</v>
       </c>
@@ -4220,7 +4239,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="9" t="s">
         <v>108</v>
       </c>
@@ -4228,7 +4247,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="9" t="s">
         <v>109</v>
       </c>
@@ -4236,7 +4255,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="9" t="s">
         <v>110</v>
       </c>
@@ -4244,17 +4263,17 @@
         <v>0.221</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="15"/>
     </row>
-    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="15" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="22"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="12" t="s">
         <v>94</v>
       </c>
@@ -4262,7 +4281,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="12" t="s">
         <v>95</v>
       </c>
@@ -4270,7 +4289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="12" t="s">
         <v>96</v>
       </c>
@@ -4278,7 +4297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="12" t="s">
         <v>97</v>
       </c>
@@ -4286,7 +4305,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="12" t="s">
         <v>98</v>
       </c>
@@ -4295,15 +4314,15 @@
         <v>0.19999999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="15"/>
     </row>
-    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="15" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="27" t="s">
         <v>101</v>
       </c>
@@ -4311,7 +4330,7 @@
         <v>0.127</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="27" t="s">
         <v>102</v>
       </c>
@@ -4319,7 +4338,7 @@
         <v>0.45200000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="27" t="s">
         <v>103</v>
       </c>
@@ -4327,7 +4346,7 @@
         <v>0.33400000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="27" t="s">
         <v>104</v>
       </c>
@@ -4335,18 +4354,18 @@
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="27"/>
       <c r="C26" s="27"/>
     </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
     </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="41" t="s">
         <v>75</v>
       </c>
@@ -4354,7 +4373,7 @@
         <v>0.20799999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="41" t="s">
         <v>76</v>
       </c>
@@ -4362,7 +4381,7 @@
         <v>0.63700000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="41" t="s">
         <v>77</v>
       </c>
@@ -4370,7 +4389,7 @@
         <v>0.11899999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="41" t="s">
         <v>78</v>
       </c>
@@ -4378,7 +4397,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B32" s="45" t="s">
         <v>130</v>
       </c>
@@ -4387,20 +4406,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B35" s="9"/>
       <c r="C35" s="16"/>
     </row>
-    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="60" t="s">
         <v>92</v>
       </c>
@@ -4408,7 +4427,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="19" t="s">
         <v>91</v>
       </c>
@@ -4418,7 +4437,7 @@
       <c r="D37" s="20"/>
       <c r="E37" s="21"/>
     </row>
-    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="19" t="s">
         <v>90</v>
       </c>
@@ -4428,7 +4447,7 @@
       <c r="D38" s="20"/>
       <c r="E38" s="20"/>
     </row>
-    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="19" t="s">
         <v>172</v>
       </c>
@@ -4436,7 +4455,7 @@
         <v>4.01</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B40" s="19" t="s">
         <v>89</v>
       </c>
@@ -4444,7 +4463,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" s="60" t="s">
         <v>93</v>
       </c>
@@ -4452,16 +4471,16 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D42" s="20"/>
     </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="15" t="s">
         <v>134</v>
       </c>
       <c r="D43" s="20"/>
     </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B44" s="19" t="s">
         <v>9</v>
       </c>
@@ -4470,7 +4489,7 @@
       </c>
       <c r="D44" s="20"/>
     </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B45" s="19" t="s">
         <v>11</v>
       </c>
@@ -4479,7 +4498,7 @@
       </c>
       <c r="D45" s="20"/>
     </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B46" s="19" t="s">
         <v>12</v>
       </c>
@@ -4489,7 +4508,7 @@
       <c r="D46" s="20"/>
       <c r="E46" s="21"/>
     </row>
-    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B47" s="19" t="s">
         <v>26</v>
       </c>
@@ -4500,16 +4519,16 @@
       <c r="D47" s="20"/>
       <c r="E47" s="20"/>
     </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D48" s="20"/>
     </row>
-    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="15" t="s">
         <v>72</v>
       </c>
       <c r="D49" s="20"/>
     </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B50" s="19" t="s">
         <v>125</v>
       </c>
@@ -4518,7 +4537,7 @@
       </c>
       <c r="D50" s="20"/>
     </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B51" s="19" t="s">
         <v>126</v>
       </c>
@@ -4526,7 +4545,7 @@
         <v>1.66</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B52" s="19" t="s">
         <v>127</v>
       </c>
@@ -4534,7 +4553,7 @@
         <v>5.64</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B53" s="19" t="s">
         <v>128</v>
       </c>
@@ -4542,7 +4561,7 @@
         <v>5.43</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B54" s="19" t="s">
         <v>129</v>
       </c>
@@ -4550,12 +4569,12 @@
         <v>1.91</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="15" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B57" s="9" t="s">
         <v>111</v>
       </c>
@@ -4563,7 +4582,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B58" s="19" t="s">
         <v>133</v>
       </c>
@@ -4571,7 +4590,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="4"/>
     </row>
   </sheetData>
@@ -4581,7 +4600,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -4591,117 +4610,117 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" style="80" customWidth="1"/>
-    <col min="2" max="16384" width="10.85546875" style="80"/>
+    <col min="1" max="1" width="18.6640625" style="75" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="75"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
-        <v>198</v>
-      </c>
-      <c r="B1" s="84" t="s">
+    <row r="1" spans="1:5" ht="40" x14ac:dyDescent="0.2">
+      <c r="A1" s="80" t="s">
+        <v>197</v>
+      </c>
+      <c r="B1" s="79" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="84" t="s">
+      <c r="C1" s="79" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="84" t="s">
+      <c r="D1" s="79" t="s">
         <v>176</v>
       </c>
-      <c r="E1" s="84" t="s">
+      <c r="E1" s="79" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="83" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="78" t="s">
         <v>165</v>
       </c>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="72">
+      <c r="C2" s="70">
         <f>1.5*0.61</f>
         <v>0.91500000000000004</v>
       </c>
-      <c r="D2" s="72">
+      <c r="D2" s="70">
         <v>3.78</v>
       </c>
-      <c r="E2" s="72">
+      <c r="E2" s="70">
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="82"/>
-      <c r="B3" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="72">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="77"/>
+      <c r="B3" s="77" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="70">
         <f>1.5*0.61</f>
         <v>0.91500000000000004</v>
       </c>
-      <c r="D3" s="72">
+      <c r="D3" s="70">
         <f t="shared" ref="D3:D6" si="0">10.49/4</f>
         <v>2.6225000000000001</v>
       </c>
-      <c r="E3" s="72">
+      <c r="E3" s="70">
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="82"/>
-      <c r="B4" s="82" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="77"/>
+      <c r="B4" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="72">
+      <c r="C4" s="70">
         <f>1.5*0.61</f>
         <v>0.91500000000000004</v>
       </c>
-      <c r="D4" s="72">
+      <c r="D4" s="70">
         <f t="shared" si="0"/>
         <v>2.6225000000000001</v>
       </c>
-      <c r="E4" s="72">
+      <c r="E4" s="70">
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="82"/>
-      <c r="B5" s="82" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="77"/>
+      <c r="B5" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="72">
+      <c r="C5" s="70">
         <f>1.5*0.61</f>
         <v>0.91500000000000004</v>
       </c>
-      <c r="D5" s="72">
+      <c r="D5" s="70">
         <f t="shared" si="0"/>
         <v>2.6225000000000001</v>
       </c>
-      <c r="E5" s="72">
+      <c r="E5" s="70">
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="82"/>
-      <c r="B6" s="82" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="77"/>
+      <c r="B6" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="72">
+      <c r="C6" s="70">
         <f>1.5*0.61</f>
         <v>0.91500000000000004</v>
       </c>
-      <c r="D6" s="72">
+      <c r="D6" s="70">
         <f t="shared" si="0"/>
         <v>2.6225000000000001</v>
       </c>
-      <c r="E6" s="72">
+      <c r="E6" s="70">
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="81"/>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C9" s="76"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4709,7 +4728,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -4719,15 +4738,15 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="53" style="70" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.85546875" style="53" customWidth="1"/>
-    <col min="3" max="3" width="42.42578125" style="53" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="53"/>
+    <col min="1" max="1" width="53" style="68" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.83203125" style="53" customWidth="1"/>
+    <col min="3" max="3" width="42.5" style="53" customWidth="1"/>
+    <col min="4" max="16384" width="11.5" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="58" t="s">
         <v>69</v>
       </c>
@@ -4738,64 +4757,64 @@
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="66"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C2" s="64"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="66"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="70" t="s">
+      <c r="C3" s="64"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="C4" s="66"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="70" t="s">
+      <c r="C4" s="64"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" s="68" t="s">
         <v>138</v>
       </c>
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="C5" s="66"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C5" s="64"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="49"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" s="49"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="49"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="49"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="49"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="49"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" s="49"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" s="49"/>
     </row>
   </sheetData>
@@ -4806,7 +4825,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -4816,86 +4835,86 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="30.140625" style="53" customWidth="1"/>
-    <col min="2" max="16384" width="11.42578125" style="53"/>
+    <col min="1" max="1" width="30.1640625" style="53" customWidth="1"/>
+    <col min="2" max="16384" width="11.5" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="58" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="66" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="66" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2" s="64" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A3" s="64" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="66" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A4" s="64" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="66" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5" s="64" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="66" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A6" s="64" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="66" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A7" s="64" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="66" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A8" s="64" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="66" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A9" s="64" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="66"/>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="66"/>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="66"/>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="66"/>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="66"/>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="66"/>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="66"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="66"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="66"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="66"/>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A10" s="64"/>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A11" s="64"/>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A12" s="64"/>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A13" s="64"/>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A14" s="64"/>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A15" s="64"/>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A16" s="64"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A17" s="64"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A18" s="64"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A19" s="64"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4904,7 +4923,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.34998626667073579"/>
   </sheetPr>
@@ -4914,9 +4933,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -4936,7 +4955,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>71</v>
       </c>
@@ -4961,7 +4980,7 @@
         <v>1.91</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>65</v>
       </c>
@@ -4986,7 +5005,7 @@
         <v>5.8059717622450747E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>66</v>
       </c>
@@ -5018,29 +5037,29 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.85546875" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.83203125" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -5087,7 +5106,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>31</v>
       </c>
@@ -5138,7 +5157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="9" t="s">
         <v>150</v>
       </c>
@@ -5182,9 +5201,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C4" s="51">
         <v>1</v>
@@ -5226,7 +5245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="14" t="s">
         <v>137</v>
       </c>
@@ -5272,7 +5291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="14" t="s">
         <v>138</v>
       </c>
@@ -5319,24 +5338,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="49" t="s">
         <v>84</v>
       </c>
       <c r="C7" s="51">
-        <v>1</v>
+        <f>diarrhoea_1mo/26</f>
+        <v>6.3846153846153844E-2</v>
       </c>
       <c r="D7" s="51">
-        <v>1</v>
+        <f>diarrhoea_1_5mo/26</f>
+        <v>6.3846153846153844E-2</v>
       </c>
       <c r="E7" s="51">
-        <v>1</v>
+        <f>diarrhoea_6_11mo/26</f>
+        <v>0.21692307692307691</v>
       </c>
       <c r="F7" s="51">
-        <v>1</v>
+        <f>diarrhoea_12_23mo/26</f>
+        <v>0.20884615384615385</v>
       </c>
       <c r="G7" s="51">
-        <v>1</v>
+        <f>diarrhoea_24_59mo/26</f>
+        <v>7.3461538461538453E-2</v>
       </c>
       <c r="H7" s="52">
         <v>0</v>
@@ -5363,7 +5387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="14" t="s">
         <v>58</v>
       </c>
@@ -5409,7 +5433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="14" t="s">
         <v>67</v>
       </c>
@@ -5457,7 +5481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="14" t="s">
         <v>28</v>
       </c>
@@ -5501,24 +5525,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="49" t="s">
         <v>85</v>
       </c>
       <c r="C11" s="51">
-        <v>1</v>
+        <f>diarrhoea_1mo/26</f>
+        <v>6.3846153846153844E-2</v>
       </c>
       <c r="D11" s="51">
-        <v>1</v>
+        <f>diarrhoea_1_5mo/26</f>
+        <v>6.3846153846153844E-2</v>
       </c>
       <c r="E11" s="51">
-        <v>1</v>
+        <f>diarrhoea_6_11mo/26</f>
+        <v>0.21692307692307691</v>
       </c>
       <c r="F11" s="51">
-        <v>1</v>
+        <f>diarrhoea_12_23mo/26</f>
+        <v>0.20884615384615385</v>
       </c>
       <c r="G11" s="51">
-        <v>1</v>
+        <f>diarrhoea_24_59mo/26</f>
+        <v>7.3461538461538453E-2</v>
       </c>
       <c r="H11" s="52">
         <v>0</v>
@@ -5545,7 +5574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="14" t="s">
         <v>60</v>
       </c>
@@ -5589,10 +5618,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="49"/>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -5643,7 +5672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4"/>
       <c r="B15" s="14" t="s">
         <v>86</v>
@@ -5688,7 +5717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4"/>
       <c r="B16" s="14" t="s">
         <v>188</v>
@@ -5737,7 +5766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4"/>
       <c r="B17" s="14" t="s">
         <v>193</v>
@@ -5786,7 +5815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="49" t="s">
         <v>57</v>
       </c>
@@ -5834,7 +5863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="14" t="s">
         <v>88</v>
       </c>
@@ -5878,7 +5907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="14" t="s">
         <v>87</v>
       </c>
@@ -5922,7 +5951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="49" t="s">
         <v>59</v>
       </c>
@@ -5970,15 +5999,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="49"/>
     </row>
-    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="87" t="s">
+    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="89" t="s">
-        <v>201</v>
+      <c r="B23" s="83" t="s">
+        <v>200</v>
       </c>
       <c r="C23" s="52">
         <v>0</v>
@@ -6020,8 +6049,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="89" t="s">
+    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B24" s="83" t="s">
         <v>189</v>
       </c>
       <c r="C24" s="52">
@@ -6068,8 +6097,8 @@
         <v>0.54921999999999993</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="89" t="s">
+    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" s="83" t="s">
         <v>190</v>
       </c>
       <c r="C25" s="52">
@@ -6116,8 +6145,8 @@
         <v>0.23537999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="89" t="s">
+    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B26" s="83" t="s">
         <v>191</v>
       </c>
       <c r="C26" s="52">
@@ -6164,8 +6193,8 @@
         <v>0.21539999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="89" t="s">
+    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B27" s="83" t="s">
         <v>192</v>
       </c>
       <c r="C27" s="52">
@@ -6209,7 +6238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="14"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -6219,7 +6248,7 @@
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
     </row>
-    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
         <v>35</v>
       </c>
@@ -6277,7 +6306,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="14" t="s">
         <v>64</v>
       </c>
@@ -6332,7 +6361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="14" t="s">
         <v>62</v>
       </c>
@@ -6387,7 +6416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="14" t="s">
         <v>47</v>
       </c>
@@ -6431,7 +6460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" s="14" t="s">
         <v>34</v>
       </c>
@@ -6488,7 +6517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B34" s="49" t="s">
         <v>83</v>
       </c>
@@ -6532,7 +6561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="5"/>
       <c r="B35" s="49" t="s">
         <v>82</v>
@@ -6577,7 +6606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="49" t="s">
         <v>81</v>
       </c>
@@ -6621,7 +6650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="49" t="s">
         <v>79</v>
       </c>
@@ -6665,7 +6694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="49" t="s">
         <v>80</v>
       </c>
@@ -6709,7 +6738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="49"/>
     </row>
   </sheetData>
@@ -6722,7 +6751,45 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA98797-1B50-1C46-868B-824E5FEAF95C}">
+  <sheetPr>
+    <tabColor theme="0" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1" s="15" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2" s="15" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A3" s="15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A4" s="15" t="s">
+        <v>207</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -6732,16 +6799,16 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" style="53" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="53" customWidth="1"/>
-    <col min="3" max="4" width="11.42578125" style="53"/>
-    <col min="5" max="5" width="17.42578125" style="53" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="53"/>
+    <col min="1" max="1" width="33.6640625" style="53" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="53" customWidth="1"/>
+    <col min="3" max="4" width="11.5" style="53"/>
+    <col min="5" max="5" width="17.5" style="53" customWidth="1"/>
+    <col min="6" max="16384" width="11.5" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="58" t="s">
         <v>164</v>
       </c>
@@ -6758,7 +6825,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="57" t="s">
         <v>159</v>
       </c>
@@ -6776,7 +6843,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="57" t="s">
         <v>158</v>
       </c>
@@ -6794,7 +6861,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="57" t="s">
         <v>157</v>
       </c>
@@ -6812,7 +6879,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="57" t="s">
         <v>156</v>
       </c>
@@ -6830,7 +6897,7 @@
         <v>0.126</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="57" t="s">
         <v>155</v>
       </c>
@@ -6848,7 +6915,7 @@
         <v>1.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="57" t="s">
         <v>154</v>
       </c>
@@ -6866,7 +6933,7 @@
         <v>0.40500000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="57" t="s">
         <v>153</v>
       </c>
@@ -6884,7 +6951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="57" t="s">
         <v>152</v>
       </c>
@@ -6902,7 +6969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="57" t="s">
         <v>151</v>
       </c>
@@ -6920,7 +6987,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C11" s="54"/>
     </row>
   </sheetData>
@@ -6931,24 +6998,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" style="15" customWidth="1"/>
-    <col min="2" max="10" width="16.85546875" style="15" customWidth="1"/>
-    <col min="11" max="16384" width="14.42578125" style="15"/>
+    <col min="1" max="1" width="8.5" style="15" customWidth="1"/>
+    <col min="2" max="10" width="16.83203125" style="15" customWidth="1"/>
+    <col min="11" max="16384" width="14.5" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
@@ -6980,7 +7047,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="9">
         <f>start_year</f>
         <v>2017</v>
@@ -7016,7 +7083,7 @@
         <v>10889222.411291081</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9">
         <f t="shared" ref="A3:A40" si="1">IF($A$2+ROW(A3)-2&lt;=end_year,A2+1,"")</f>
         <v>2018</v>
@@ -7052,7 +7119,7 @@
         <v>11314876.916718401</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9">
         <f t="shared" si="1"/>
         <v>2019</v>
@@ -7088,7 +7155,7 @@
         <v>11742062.79850255</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="9">
         <f t="shared" si="1"/>
         <v>2020</v>
@@ -7124,7 +7191,7 @@
         <v>12188008.303929869</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="9">
         <f t="shared" si="1"/>
         <v>2021</v>
@@ -7160,7 +7227,7 @@
         <v>12645913.809357187</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="9">
         <f t="shared" si="1"/>
         <v>2022</v>
@@ -7196,7 +7263,7 @@
         <v>13098634.691141337</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="9">
         <f t="shared" si="1"/>
         <v>2023</v>
@@ -7232,7 +7299,7 @@
         <v>13560643.572925486</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9">
         <f t="shared" si="1"/>
         <v>2024</v>
@@ -7268,7 +7335,7 @@
         <v>14048879.078352805</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="9">
         <f t="shared" si="1"/>
         <v>2025</v>
@@ -7304,7 +7371,7 @@
         <v>14530354.336493783</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="9">
         <f t="shared" si="1"/>
         <v>2026</v>
@@ -7340,7 +7407,7 @@
         <v>15032265.218277931</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9">
         <f t="shared" si="1"/>
         <v>2027</v>
@@ -7376,7 +7443,7 @@
         <v>15550202.10006208</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9">
         <f t="shared" si="1"/>
         <v>2028</v>
@@ -7412,7 +7479,7 @@
         <v>16082324.981846228</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9">
         <f t="shared" si="1"/>
         <v>2029</v>
@@ -7448,7 +7515,7 @@
         <v>16613455.239987208</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9">
         <f t="shared" si="1"/>
         <v>2030</v>
@@ -7484,7 +7551,7 @@
         <v>17165139.121771358</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7508,7 +7575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7531,8 +7598,9 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L17" s="20"/>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7556,7 +7624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7580,7 +7648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7604,7 +7672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7628,7 +7696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7652,7 +7720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7676,7 +7744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7700,7 +7768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7724,7 +7792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7748,7 +7816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7772,7 +7840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7796,7 +7864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7820,7 +7888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7844,7 +7912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7868,7 +7936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7892,7 +7960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7916,7 +7984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7940,7 +8008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7964,7 +8032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7988,7 +8056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8012,7 +8080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8036,7 +8104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8060,7 +8128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8096,7 +8164,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -8106,13 +8174,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" customWidth="1"/>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
     <col min="2" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="str">
         <f>"Percentage of deaths in baseline year ("&amp;start_year&amp;") attributable to cause"</f>
         <v>Percentage of deaths in baseline year (2017) attributable to cause</v>
@@ -8136,7 +8204,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="32" t="s">
         <v>73</v>
       </c>
@@ -8159,7 +8227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="32" t="s">
         <v>7</v>
       </c>
@@ -8182,7 +8250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="32" t="s">
         <v>8</v>
       </c>
@@ -8205,7 +8273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="32" t="s">
         <v>10</v>
       </c>
@@ -8228,7 +8296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="32" t="s">
         <v>13</v>
       </c>
@@ -8251,7 +8319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="32" t="s">
         <v>14</v>
       </c>
@@ -8274,7 +8342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="32" t="s">
         <v>27</v>
       </c>
@@ -8297,7 +8365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="32" t="s">
         <v>15</v>
       </c>
@@ -8320,7 +8388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="32" t="s">
         <v>71</v>
       </c>
@@ -8343,7 +8411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="32" t="s">
         <v>16</v>
       </c>
@@ -8366,7 +8434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="32" t="s">
         <v>17</v>
       </c>
@@ -8389,7 +8457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="32" t="s">
         <v>18</v>
       </c>
@@ -8412,7 +8480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="32" t="s">
         <v>19</v>
       </c>
@@ -8435,7 +8503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="32" t="s">
         <v>20</v>
       </c>
@@ -8458,7 +8526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="32" t="s">
         <v>21</v>
       </c>
@@ -8481,7 +8549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="32" t="s">
         <v>22</v>
       </c>
@@ -8504,7 +8572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="32" t="s">
         <v>23</v>
       </c>
@@ -8527,7 +8595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="32" t="s">
         <v>38</v>
       </c>
@@ -8550,7 +8618,7 @@
         <v>0.10082724000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="32" t="s">
         <v>39</v>
       </c>
@@ -8573,7 +8641,7 @@
         <v>3.1206000000000002E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="32" t="s">
         <v>40</v>
       </c>
@@ -8596,7 +8664,7 @@
         <v>0.15891214000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="32" t="s">
         <v>41</v>
       </c>
@@ -8619,7 +8687,7 @@
         <v>0.12598688999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="32" t="s">
         <v>42</v>
       </c>
@@ -8642,7 +8710,7 @@
         <v>0.12434007</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="32" t="s">
         <v>43</v>
       </c>
@@ -8665,7 +8733,7 @@
         <v>3.9028409999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="32" t="s">
         <v>44</v>
       </c>
@@ -8688,7 +8756,7 @@
         <v>8.5254999999999999E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="32" t="s">
         <v>45</v>
       </c>
@@ -8711,7 +8779,7 @@
         <v>6.8467810000000004E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="32" t="s">
         <v>46</v>
       </c>
@@ -8742,7 +8810,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -8752,13 +8820,13 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.5" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="38" t="str">
         <f>"Percentage of population in each category in baseline year ("&amp;start_year&amp;")"</f>
         <v>Percentage of population in each category in baseline year (2017)</v>
@@ -8782,7 +8850,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>116</v>
       </c>
@@ -8810,33 +8878,33 @@
         <v>0.23269074767298425</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5"/>
       <c r="B3" s="14" t="s">
         <v>119</v>
       </c>
       <c r="C3" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(C4:C5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE) - SUM(C4:C5), "")</f>
         <v>0.32228430019523346</v>
       </c>
       <c r="D3" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(D4:D5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5), 0, 1) + 1, 0, 1, TRUE) - SUM(D4:D5), "")</f>
         <v>0.32228430019523346</v>
       </c>
       <c r="E3" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E4:E5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(E4:E5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E4:E5), 0, 1) + 1, 0, 1, TRUE) - SUM(E4:E5), "")</f>
         <v>0.35908666207150708</v>
       </c>
       <c r="F3" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F4:F5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(F4:F5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F4:F5), 0, 1) + 1, 0, 1, TRUE) - SUM(F4:F5), "")</f>
         <v>0.37651189492768178</v>
       </c>
       <c r="G3" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G4:G5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(G4:G5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G4:G5), 0, 1) + 1, 0, 1, TRUE) - SUM(G4:G5), "")</f>
         <v>0.37372365733745416</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5"/>
       <c r="B4" s="14" t="s">
         <v>117</v>
@@ -8857,7 +8925,7 @@
         <v>0.25929610299234518</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5"/>
       <c r="B5" s="14" t="s">
         <v>120</v>
@@ -8878,7 +8946,7 @@
         <v>0.13428949199721643</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="17"/>
       <c r="C6" s="40"/>
       <c r="D6" s="40"/>
@@ -8886,7 +8954,7 @@
       <c r="F6" s="40"/>
       <c r="G6" s="40"/>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="17"/>
       <c r="C7" s="40"/>
       <c r="D7" s="40"/>
@@ -8894,7 +8962,7 @@
       <c r="F7" s="40"/>
       <c r="G7" s="40"/>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>115</v>
       </c>
@@ -8922,32 +8990,32 @@
         <v>0.81212055177975573</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="9" t="s">
         <v>122</v>
       </c>
       <c r="C9" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(C10:C11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE) - SUM(C10:C11), "")</f>
         <v>0.28180440984664923</v>
       </c>
       <c r="D9" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D10:D11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(D10:D11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D10:D11), 0, 1) + 1, 0, 1, TRUE) - SUM(D10:D11), "")</f>
         <v>0.28180440984664923</v>
       </c>
       <c r="E9" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E10:E11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(E10:E11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E10:E11), 0, 1) + 1, 0, 1, TRUE) - SUM(E10:E11), "")</f>
         <v>0.2466938696379041</v>
       </c>
       <c r="F9" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F10:F11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(F10:F11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F10:F11), 0, 1) + 1, 0, 1, TRUE) - SUM(F10:F11), "")</f>
         <v>0.21506846670192739</v>
       </c>
       <c r="G9" s="46">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G10:G11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(G10:G11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G10:G11), 0, 1) + 1, 0, 1, TRUE) - SUM(G10:G11), "")</f>
         <v>0.15821429221536368</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="9" t="s">
         <v>123</v>
       </c>
@@ -8967,7 +9035,7 @@
         <v>2.2330660624019519E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="9" t="s">
         <v>124</v>
       </c>
@@ -8987,7 +9055,7 @@
         <v>7.3344953808610778E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -9001,7 +9069,7 @@
       <c r="N12" s="18"/>
       <c r="O12" s="18"/>
     </row>
-    <row r="13" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="15" t="s">
         <v>70</v>
       </c>
@@ -9045,7 +9113,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="19" t="s">
         <v>132</v>
       </c>
@@ -9089,7 +9157,7 @@
         <v>0.442</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="19" t="s">
         <v>68</v>
       </c>
@@ -9146,14 +9214,14 @@
         <v>0.18564</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -9168,23 +9236,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" customWidth="1"/>
-    <col min="2" max="7" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" customWidth="1"/>
+    <col min="2" max="7" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="38" t="str">
         <f>"Percentage of children in each category in baseline year ("&amp;start_year&amp;")"</f>
         <v>Percentage of children in each category in baseline year (2017)</v>
@@ -9208,7 +9276,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -9231,7 +9299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B3" s="61" t="s">
         <v>168</v>
       </c>
@@ -9251,7 +9319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B4" s="61" t="s">
         <v>169</v>
       </c>
@@ -9271,7 +9339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B5" s="61" t="s">
         <v>170</v>
       </c>
@@ -9302,7 +9370,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -9312,13 +9380,13 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>139</v>
       </c>
@@ -9353,7 +9421,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>140</v>
       </c>
@@ -9370,10 +9438,10 @@
       <c r="J2" s="39"/>
       <c r="K2" s="39"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B3" s="17"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>141</v>
       </c>
@@ -9390,10 +9458,10 @@
       <c r="J4" s="39"/>
       <c r="K4" s="39"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B5" s="17"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>142</v>
       </c>
@@ -9410,7 +9478,7 @@
       <c r="J6" s="39"/>
       <c r="K6" s="39"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B7" s="17" t="s">
         <v>32</v>
       </c>
@@ -9424,7 +9492,7 @@
       <c r="J7" s="39"/>
       <c r="K7" s="39"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B8" s="17" t="s">
         <v>145</v>
       </c>
@@ -9438,7 +9506,7 @@
       <c r="J8" s="39"/>
       <c r="K8" s="39"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>143</v>
       </c>
@@ -9455,7 +9523,7 @@
       <c r="J10" s="39"/>
       <c r="K10" s="39"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B11" s="50" t="s">
         <v>147</v>
       </c>
@@ -9469,7 +9537,7 @@
       <c r="J11" s="39"/>
       <c r="K11" s="39"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13" s="15" t="s">
         <v>74</v>
       </c>
@@ -9486,7 +9554,7 @@
       <c r="J13" s="39"/>
       <c r="K13" s="39"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B14" s="19" t="s">
         <v>171</v>
       </c>
@@ -9507,273 +9575,287 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17" style="53" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" style="53" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="53" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="53"/>
+    <col min="2" max="2" width="19.1640625" style="53" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="53" customWidth="1"/>
+    <col min="4" max="16384" width="11.5" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="68" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A1" s="66" t="s">
         <v>179</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="67" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="67" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="67" t="s">
         <v>176</v>
       </c>
-      <c r="E1" s="69" t="s">
+      <c r="E1" s="67" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="67" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A2" s="65" t="s">
         <v>174</v>
       </c>
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="86" t="str">
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="65"/>
-      <c r="B3" s="64" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="66" t="s">
-        <v>197</v>
-      </c>
-      <c r="D3" s="66"/>
-      <c r="E3" s="86" t="str">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="63"/>
+      <c r="B3" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="89" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="89"/>
+      <c r="E3" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="65"/>
-      <c r="B4" s="64" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="63"/>
+      <c r="B4" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="66" t="s">
-        <v>197</v>
-      </c>
-      <c r="D4" s="66"/>
-      <c r="E4" s="86" t="str">
+      <c r="C4" s="89" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="89"/>
+      <c r="E4" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="65"/>
-      <c r="B5" s="64" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="63"/>
+      <c r="B5" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="66" t="s">
-        <v>197</v>
-      </c>
-      <c r="D5" s="66"/>
-      <c r="E5" s="86" t="str">
+      <c r="C5" s="89" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="89"/>
+      <c r="E5" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="65"/>
-      <c r="B6" s="64" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" s="63"/>
+      <c r="B6" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="66" t="s">
-        <v>197</v>
-      </c>
-      <c r="D6" s="66"/>
-      <c r="E6" s="86" t="str">
+      <c r="C6" s="89" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="89"/>
+      <c r="E6" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="65"/>
-      <c r="B7" s="64" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" s="63"/>
+      <c r="B7" s="62" t="s">
         <v>173</v>
       </c>
-      <c r="C7" s="63"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="66"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="67" t="s">
-        <v>202</v>
-      </c>
-      <c r="B9" s="64" t="s">
+      <c r="C7" s="91"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="89"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="C8" s="93"/>
+      <c r="D8" s="93"/>
+      <c r="E8" s="93"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A9" s="65" t="s">
+        <v>201</v>
+      </c>
+      <c r="B9" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="66"/>
-      <c r="D9" s="66" t="s">
-        <v>197</v>
-      </c>
-      <c r="E9" s="86" t="str">
+      <c r="C9" s="89"/>
+      <c r="D9" s="89"/>
+      <c r="E9" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="65"/>
-      <c r="B10" s="64" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="66"/>
-      <c r="D10" s="66"/>
-      <c r="E10" s="86" t="str">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A10" s="63"/>
+      <c r="B10" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="89" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" s="89"/>
+      <c r="E10" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="65"/>
-      <c r="B11" s="64" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A11" s="63"/>
+      <c r="B11" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="66"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="86" t="str">
+      <c r="C11" s="89" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" s="89"/>
+      <c r="E11" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="65"/>
-      <c r="B12" s="64" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" s="63"/>
+      <c r="B12" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="66"/>
-      <c r="D12" s="66"/>
-      <c r="E12" s="86" t="str">
+      <c r="C12" s="89" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="89"/>
+      <c r="E12" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="65"/>
-      <c r="B13" s="64" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" s="63"/>
+      <c r="B13" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="86" t="str">
+      <c r="C13" s="89" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" s="89"/>
+      <c r="E13" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="65"/>
-      <c r="B14" s="64" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="63"/>
+      <c r="B14" s="62" t="s">
         <v>173</v>
       </c>
-      <c r="C14" s="63"/>
-      <c r="D14" s="62"/>
-      <c r="E14" s="66"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="67" t="s">
-        <v>203</v>
-      </c>
-      <c r="B16" s="64" t="s">
+      <c r="C14" s="91"/>
+      <c r="D14" s="92"/>
+      <c r="E14" s="89"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="C15" s="93"/>
+      <c r="D15" s="93"/>
+      <c r="E15" s="93"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A16" s="65" t="s">
+        <v>202</v>
+      </c>
+      <c r="B16" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66" t="s">
-        <v>197</v>
-      </c>
-      <c r="E16" s="86" t="str">
+      <c r="C16" s="89"/>
+      <c r="D16" s="89"/>
+      <c r="E16" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="65"/>
-      <c r="B17" s="64" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="66"/>
-      <c r="D17" s="66" t="s">
-        <v>197</v>
-      </c>
-      <c r="E17" s="86" t="str">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A17" s="63"/>
+      <c r="B17" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="89" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="89"/>
+      <c r="E17" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="65"/>
-      <c r="B18" s="64" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18" s="63"/>
+      <c r="B18" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66" t="s">
-        <v>197</v>
-      </c>
-      <c r="E18" s="86" t="str">
+      <c r="C18" s="89" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" s="89"/>
+      <c r="E18" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="65"/>
-      <c r="B19" s="64" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19" s="63"/>
+      <c r="B19" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="66"/>
-      <c r="D19" s="66" t="s">
-        <v>197</v>
-      </c>
-      <c r="E19" s="86" t="str">
+      <c r="C19" s="89" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="89"/>
+      <c r="E19" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="65"/>
-      <c r="B20" s="64" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A20" s="63"/>
+      <c r="B20" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="66"/>
-      <c r="D20" s="66" t="s">
-        <v>197</v>
-      </c>
-      <c r="E20" s="86" t="str">
+      <c r="C20" s="89" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" s="89"/>
+      <c r="E20" s="90" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="65"/>
-      <c r="B21" s="64" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A21" s="63"/>
+      <c r="B21" s="62" t="s">
         <v>173</v>
       </c>
-      <c r="C21" s="63"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="66"/>
+      <c r="C21" s="91"/>
+      <c r="D21" s="92"/>
+      <c r="E21" s="89"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9782,61 +9864,61 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="90" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A1" s="84" t="s">
         <v>165</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="67" t="s">
         <v>182</v>
       </c>
-      <c r="C1" s="91" t="s">
+      <c r="C1" s="85" t="s">
         <v>183</v>
       </c>
-      <c r="D1" s="91" t="s">
+      <c r="D1" s="85" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="91" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="62" t="s">
         <v>184</v>
       </c>
-      <c r="D2" s="66"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="91" t="s">
+      <c r="D2" s="89"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" s="85" t="s">
         <v>186</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="62" t="s">
         <v>177</v>
       </c>
-      <c r="C3" s="64" t="s">
+      <c r="C3" s="62" t="s">
         <v>185</v>
       </c>
-      <c r="D3" s="66"/>
+      <c r="D3" s="89"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9844,535 +9926,629 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="56" style="70" customWidth="1"/>
+    <col min="1" max="1" width="56" style="68" customWidth="1"/>
     <col min="2" max="2" width="20" style="54" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" style="53" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" style="53" customWidth="1"/>
-    <col min="5" max="16384" width="14.42578125" style="53"/>
+    <col min="3" max="3" width="20.5" style="53" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" style="53" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" style="53" customWidth="1"/>
+    <col min="6" max="16384" width="14.5" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+    <row r="1" spans="1:5" ht="39" x14ac:dyDescent="0.15">
+      <c r="A1" s="74" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="94" t="str">
+      <c r="B1" s="88" t="str">
         <f>"Baseline ("&amp;start_year&amp;") coverage"</f>
         <v>Baseline (2017) coverage</v>
       </c>
-      <c r="C1" s="78" t="s">
+      <c r="C1" s="73" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1" s="72" t="s">
         <v>204</v>
       </c>
-      <c r="D1" s="77" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="70" t="s">
+      <c r="E1" s="73" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="71">
-        <v>0</v>
-      </c>
-      <c r="C2" s="71">
+      <c r="B2" s="69">
+        <v>0</v>
+      </c>
+      <c r="C2" s="69">
         <v>0.95</v>
       </c>
-      <c r="D2" s="72">
+      <c r="D2" s="70">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="70" t="s">
+      <c r="E2" s="70" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="68" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="71">
-        <v>0</v>
-      </c>
-      <c r="C3" s="71">
+      <c r="B3" s="69">
+        <v>0</v>
+      </c>
+      <c r="C3" s="69">
         <v>0.95</v>
       </c>
-      <c r="D3" s="72">
-        <v>1</v>
-      </c>
-      <c r="E3" s="61"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="70" t="s">
+      <c r="D3" s="70">
+        <v>1</v>
+      </c>
+      <c r="E3" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="71">
-        <v>0</v>
-      </c>
-      <c r="C4" s="71">
+      <c r="B4" s="69">
+        <v>0</v>
+      </c>
+      <c r="C4" s="69">
         <v>0.95</v>
       </c>
-      <c r="D4" s="72">
+      <c r="D4" s="70">
         <v>90</v>
       </c>
-      <c r="E4" s="61"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="70" t="s">
-        <v>201</v>
-      </c>
-      <c r="B5" s="71">
-        <v>0</v>
-      </c>
-      <c r="C5" s="71">
+      <c r="E4" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="68" t="s">
+        <v>200</v>
+      </c>
+      <c r="B5" s="69">
+        <v>0</v>
+      </c>
+      <c r="C5" s="69">
         <v>0.95</v>
       </c>
-      <c r="D5" s="73">
+      <c r="D5" s="71">
         <f>SUM('Programs family planning'!E2:E10)</f>
         <v>0.82100000000000006</v>
       </c>
-      <c r="E5" s="76"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="70" t="s">
+      <c r="E5" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="71">
+      <c r="B6" s="69">
         <v>0.36</v>
       </c>
-      <c r="C6" s="71">
+      <c r="C6" s="69">
         <v>0.95</v>
       </c>
-      <c r="D6" s="72">
+      <c r="D6" s="70">
         <v>0.25</v>
       </c>
-      <c r="E6" s="75"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="89" t="s">
+      <c r="E6" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="83" t="s">
         <v>189</v>
       </c>
-      <c r="B7" s="71">
-        <v>0</v>
-      </c>
-      <c r="C7" s="71">
+      <c r="B7" s="69">
+        <v>0</v>
+      </c>
+      <c r="C7" s="69">
         <v>0.95</v>
       </c>
-      <c r="D7" s="72">
+      <c r="D7" s="70">
         <v>0.73</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="89" t="s">
+      <c r="E7" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="83" t="s">
         <v>190</v>
       </c>
-      <c r="B8" s="71">
-        <v>0</v>
-      </c>
-      <c r="C8" s="71">
+      <c r="B8" s="69">
+        <v>0</v>
+      </c>
+      <c r="C8" s="69">
         <v>0.95</v>
       </c>
-      <c r="D8" s="72">
+      <c r="D8" s="70">
         <v>1.78</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="89" t="s">
+      <c r="E8" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="83" t="s">
         <v>191</v>
       </c>
-      <c r="B9" s="71">
-        <v>0</v>
-      </c>
-      <c r="C9" s="71">
+      <c r="B9" s="69">
+        <v>0</v>
+      </c>
+      <c r="C9" s="69">
         <v>0.95</v>
       </c>
-      <c r="D9" s="72">
+      <c r="D9" s="70">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="89" t="s">
+      <c r="E9" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="83" t="s">
         <v>192</v>
       </c>
-      <c r="B10" s="71">
-        <v>0</v>
-      </c>
-      <c r="C10" s="71">
+      <c r="B10" s="69">
+        <v>0</v>
+      </c>
+      <c r="C10" s="69">
         <v>0.95</v>
       </c>
-      <c r="D10" s="72">
+      <c r="D10" s="70">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E10" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="B11" s="71">
-        <v>0</v>
-      </c>
-      <c r="C11" s="71">
+      <c r="B11" s="69">
+        <v>0</v>
+      </c>
+      <c r="C11" s="69">
         <v>0.95</v>
       </c>
-      <c r="D11" s="72">
+      <c r="D11" s="70">
         <v>0.73</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E11" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="B12" s="71">
-        <v>0</v>
-      </c>
-      <c r="C12" s="71">
+      <c r="B12" s="69">
+        <v>0</v>
+      </c>
+      <c r="C12" s="69">
         <v>0.95</v>
       </c>
-      <c r="D12" s="72">
+      <c r="D12" s="70">
         <v>1.78</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="70" t="s">
+      <c r="E12" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="71">
+      <c r="B13" s="69">
         <v>0.34599999999999997</v>
       </c>
-      <c r="C13" s="71">
+      <c r="C13" s="69">
         <v>0.95</v>
       </c>
-      <c r="D13" s="72">
+      <c r="D13" s="70">
         <v>2.06</v>
       </c>
-      <c r="E13" s="61"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="70" t="s">
+      <c r="E13" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="71">
+      <c r="B14" s="69">
         <v>0.80800000000000005</v>
       </c>
-      <c r="C14" s="71">
+      <c r="C14" s="69">
         <v>0.95</v>
       </c>
-      <c r="D14" s="72">
+      <c r="D14" s="70">
         <v>0.05</v>
       </c>
-      <c r="E14" s="61"/>
-    </row>
-    <row r="15" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="70" t="s">
+      <c r="E14" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="68" t="s">
         <v>174</v>
       </c>
-      <c r="B15" s="71">
-        <v>0</v>
-      </c>
-      <c r="C15" s="71">
+      <c r="B15" s="69">
+        <v>0</v>
+      </c>
+      <c r="C15" s="69">
         <v>0.95</v>
       </c>
-      <c r="D15" s="88">
+      <c r="D15" s="82">
         <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$2:$E$6&lt;&gt;""))</f>
         <v>3.66</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="70" t="s">
+      <c r="E15" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="68" t="s">
+        <v>201</v>
+      </c>
+      <c r="B16" s="69">
+        <v>0</v>
+      </c>
+      <c r="C16" s="69">
+        <v>0.95</v>
+      </c>
+      <c r="D16" s="82">
+        <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$9:$E$13&lt;&gt;""))</f>
+        <v>3.66</v>
+      </c>
+      <c r="E16" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="68" t="s">
         <v>202</v>
       </c>
-      <c r="B16" s="71">
-        <v>0</v>
-      </c>
-      <c r="C16" s="71">
+      <c r="B17" s="69">
+        <v>0</v>
+      </c>
+      <c r="C17" s="69">
         <v>0.95</v>
       </c>
-      <c r="D16" s="88">
-        <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$9:$E$13&lt;&gt;""))</f>
+      <c r="D17" s="82">
+        <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$16:$E$20&lt;&gt;""))</f>
+        <v>3.66</v>
+      </c>
+      <c r="E17" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="68" t="s">
+        <v>198</v>
+      </c>
+      <c r="B18" s="69">
+        <v>0</v>
+      </c>
+      <c r="C18" s="69">
+        <v>0.95</v>
+      </c>
+      <c r="D18" s="70">
+        <v>8.84</v>
+      </c>
+      <c r="E18" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="68" t="s">
+        <v>137</v>
+      </c>
+      <c r="B19" s="69">
+        <v>0</v>
+      </c>
+      <c r="C19" s="69">
+        <v>0.95</v>
+      </c>
+      <c r="D19" s="70">
+        <v>50</v>
+      </c>
+      <c r="E19" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="68" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="69">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="C20" s="69">
+        <v>0.95</v>
+      </c>
+      <c r="D20" s="70">
+        <v>2.61</v>
+      </c>
+      <c r="E20" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="69">
+        <v>0</v>
+      </c>
+      <c r="C21" s="69">
+        <v>0.95</v>
+      </c>
+      <c r="D21" s="70">
+        <v>1</v>
+      </c>
+      <c r="E21" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="68" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="69">
+        <v>0</v>
+      </c>
+      <c r="C22" s="69">
+        <v>0.95</v>
+      </c>
+      <c r="D22" s="70">
+        <v>1</v>
+      </c>
+      <c r="E22" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="68" t="s">
+        <v>138</v>
+      </c>
+      <c r="B23" s="69">
+        <v>0.1</v>
+      </c>
+      <c r="C23" s="69">
+        <v>0.95</v>
+      </c>
+      <c r="D23" s="70">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="E23" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="68" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="69">
+        <v>0.3538</v>
+      </c>
+      <c r="C24" s="69">
+        <v>0.95</v>
+      </c>
+      <c r="D24" s="70">
         <v>3.78</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="70" t="s">
-        <v>203</v>
-      </c>
-      <c r="B17" s="71">
-        <v>0</v>
-      </c>
-      <c r="C17" s="71">
+      <c r="E24" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="68" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" s="69">
+        <v>0</v>
+      </c>
+      <c r="C25" s="69">
         <v>0.95</v>
       </c>
-      <c r="D17" s="88">
-        <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$16:$E$20&lt;&gt;""))</f>
-        <v>14.270000000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="70" t="s">
-        <v>199</v>
-      </c>
-      <c r="B18" s="71">
-        <v>0</v>
-      </c>
-      <c r="C18" s="71">
+      <c r="D25" s="70">
+        <v>1</v>
+      </c>
+      <c r="E25" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="69">
+        <v>0</v>
+      </c>
+      <c r="C26" s="69">
         <v>0.95</v>
       </c>
-      <c r="D18" s="72">
-        <v>8.84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="70" t="s">
-        <v>137</v>
-      </c>
-      <c r="B19" s="71">
-        <v>0</v>
-      </c>
-      <c r="C19" s="71">
+      <c r="D26" s="70">
+        <v>48</v>
+      </c>
+      <c r="E26" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="68" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="69">
+        <v>0</v>
+      </c>
+      <c r="C27" s="69">
         <v>0.95</v>
       </c>
-      <c r="D19" s="72">
-        <v>50</v>
-      </c>
-      <c r="E19" s="61"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="70" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="71">
-        <v>0.50800000000000001</v>
-      </c>
-      <c r="C20" s="71">
-        <v>0.95</v>
-      </c>
-      <c r="D20" s="72">
-        <v>2.61</v>
-      </c>
-      <c r="E20" s="61"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="70" t="s">
-        <v>88</v>
-      </c>
-      <c r="B21" s="71">
-        <v>0</v>
-      </c>
-      <c r="C21" s="71">
-        <v>0.95</v>
-      </c>
-      <c r="D21" s="72">
-        <v>1</v>
-      </c>
-      <c r="E21" s="61"/>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="70" t="s">
-        <v>87</v>
-      </c>
-      <c r="B22" s="71">
-        <v>0</v>
-      </c>
-      <c r="C22" s="71">
-        <v>0.95</v>
-      </c>
-      <c r="D22" s="72">
-        <v>1</v>
-      </c>
-      <c r="E22" s="74"/>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="70" t="s">
-        <v>138</v>
-      </c>
-      <c r="B23" s="71">
-        <v>0.1</v>
-      </c>
-      <c r="C23" s="71">
-        <v>0.95</v>
-      </c>
-      <c r="D23" s="72">
-        <v>4.6500000000000004</v>
-      </c>
-      <c r="E23" s="61"/>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="70" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24" s="71">
-        <v>0.3538</v>
-      </c>
-      <c r="C24" s="71">
-        <v>0.95</v>
-      </c>
-      <c r="D24" s="72">
-        <v>3.78</v>
-      </c>
-      <c r="E24" s="61"/>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="70" t="s">
-        <v>84</v>
-      </c>
-      <c r="B25" s="71">
-        <v>0</v>
-      </c>
-      <c r="C25" s="71">
-        <v>0.95</v>
-      </c>
-      <c r="D25" s="72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="70" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26" s="71">
-        <v>0</v>
-      </c>
-      <c r="C26" s="71">
-        <v>0.95</v>
-      </c>
-      <c r="D26" s="72">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="70" t="s">
-        <v>67</v>
-      </c>
-      <c r="B27" s="71">
-        <v>0</v>
-      </c>
-      <c r="C27" s="71">
-        <v>0.95</v>
-      </c>
-      <c r="D27" s="73">
+      <c r="D27" s="71">
         <f>90*AVERAGE('Incidence of conditions'!B4:F4) + 40*AVERAGE('Incidence of conditions'!B3:F3)*IF(ISBLANK(manage_mam), 0, 1)</f>
         <v>5.2956558655829511</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="70" t="s">
+      <c r="E27" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="71">
+      <c r="B28" s="69">
         <v>0.89970000000000006</v>
       </c>
-      <c r="C28" s="71">
+      <c r="C28" s="69">
         <v>0.95</v>
       </c>
-      <c r="D28" s="72">
+      <c r="D28" s="70">
         <v>0.41</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="70" t="s">
+      <c r="E28" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="68" t="s">
         <v>83</v>
       </c>
-      <c r="B29" s="71">
+      <c r="B29" s="69">
         <v>0.80700000000000005</v>
       </c>
-      <c r="C29" s="71">
+      <c r="C29" s="69">
         <v>0.95</v>
       </c>
-      <c r="D29" s="72">
+      <c r="D29" s="70">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="70" t="s">
+      <c r="E29" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="68" t="s">
         <v>82</v>
       </c>
-      <c r="B30" s="71">
+      <c r="B30" s="69">
         <v>0.73199999999999998</v>
       </c>
-      <c r="C30" s="71">
+      <c r="C30" s="69">
         <v>0.95</v>
       </c>
-      <c r="D30" s="72">
+      <c r="D30" s="70">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="70" t="s">
+      <c r="E30" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="68" t="s">
         <v>81</v>
       </c>
-      <c r="B31" s="71">
+      <c r="B31" s="69">
         <v>0.316</v>
       </c>
-      <c r="C31" s="71">
+      <c r="C31" s="69">
         <v>0.95</v>
       </c>
-      <c r="D31" s="72">
+      <c r="D31" s="70">
         <v>79</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="70" t="s">
+      <c r="E31" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="68" t="s">
         <v>79</v>
       </c>
-      <c r="B32" s="71">
+      <c r="B32" s="69">
         <v>0.59699999999999998</v>
       </c>
-      <c r="C32" s="71">
+      <c r="C32" s="69">
         <v>0.95</v>
       </c>
-      <c r="D32" s="72">
+      <c r="D32" s="70">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="70" t="s">
+      <c r="E32" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="68" t="s">
         <v>80</v>
       </c>
-      <c r="B33" s="71">
+      <c r="B33" s="69">
         <v>0.19900000000000001</v>
       </c>
-      <c r="C33" s="71">
+      <c r="C33" s="69">
         <v>0.95</v>
       </c>
-      <c r="D33" s="72">
+      <c r="D33" s="70">
         <v>102</v>
       </c>
+      <c r="E33" s="70" t="s">
+        <v>208</v>
+      </c>
       <c r="F33" s="53"/>
     </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="70" t="s">
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="68" t="s">
         <v>85</v>
       </c>
-      <c r="B34" s="71">
+      <c r="B34" s="69">
         <v>0.13400000000000001</v>
       </c>
-      <c r="C34" s="71">
+      <c r="C34" s="69">
         <v>0.95</v>
       </c>
-      <c r="D34" s="72">
+      <c r="D34" s="70">
         <v>5.53</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="70" t="s">
+      <c r="E34" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="B35" s="71">
-        <v>0</v>
-      </c>
-      <c r="C35" s="71">
+      <c r="B35" s="69">
+        <v>0</v>
+      </c>
+      <c r="C35" s="69">
         <v>0.95</v>
       </c>
-      <c r="D35" s="72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D35" s="70">
+        <v>1</v>
+      </c>
+      <c r="E35" s="70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F36" s="54"/>
     </row>
   </sheetData>
@@ -10381,5 +10557,17 @@
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4E3893C6-1CD6-D045-8057-77412F55397B}">
+          <x14:formula1>
+            <xm:f>'Cost curve options'!$A$1:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E35</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated template and regional books
</commit_message>
<xml_diff>
--- a/applications/demo/data/regional/demoregion1_input.xlsx
+++ b/applications/demo/data/regional/demoregion1_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/demo/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B5FFAB85-380B-6C44-9A07-35BAE6437924}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{99BDCD51-4C4B-F64C-A6D1-64A2D6F36993}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="961" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -18,66 +18,66 @@
     <sheet name="Causes of death" sheetId="4" r:id="rId3"/>
     <sheet name="Nutritional status distribution" sheetId="5" r:id="rId4"/>
     <sheet name="Breastfeeding distribution" sheetId="50" r:id="rId5"/>
-    <sheet name="Time trends" sheetId="51" r:id="rId6"/>
+    <sheet name="Time trends" sheetId="51" state="hidden" r:id="rId6"/>
     <sheet name="IYCF packages" sheetId="55" r:id="rId7"/>
     <sheet name="Treatment of SAM" sheetId="60" r:id="rId8"/>
     <sheet name="Programs cost and coverage" sheetId="56" r:id="rId9"/>
     <sheet name="IYCF cost" sheetId="57" r:id="rId10"/>
     <sheet name="Program dependencies" sheetId="58" r:id="rId11"/>
     <sheet name="Reference programs" sheetId="59" state="hidden" r:id="rId12"/>
-    <sheet name="Incidence of conditions" sheetId="7" r:id="rId13"/>
+    <sheet name="Incidence of conditions" sheetId="7" state="hidden" r:id="rId13"/>
     <sheet name="Programs target population" sheetId="21" r:id="rId14"/>
     <sheet name="Cost curve options" sheetId="61" state="hidden" r:id="rId15"/>
-    <sheet name="Programs family planning" sheetId="54" state="hidden" r:id="rId16"/>
+    <sheet name="Programs family planning" sheetId="54" r:id="rId16"/>
   </sheets>
   <definedNames>
-    <definedName name="abortion" localSheetId="6">'Baseline year population inputs'!$C$37</definedName>
-    <definedName name="abortion">'Baseline year population inputs'!$C$40</definedName>
+    <definedName name="abortion" localSheetId="6">'Baseline year population inputs'!$C$38</definedName>
+    <definedName name="abortion">'Baseline year population inputs'!$C$41</definedName>
     <definedName name="comm_deliv">'Treatment of SAM'!$D$3</definedName>
-    <definedName name="diarrhoea_1_5mo">'Baseline year population inputs'!$C$51</definedName>
-    <definedName name="diarrhoea_12_23mo">'Baseline year population inputs'!$C$53</definedName>
-    <definedName name="diarrhoea_1mo">'Baseline year population inputs'!$C$50</definedName>
-    <definedName name="diarrhoea_24_59mo">'Baseline year population inputs'!$C$54</definedName>
-    <definedName name="diarrhoea_6_11mo">'Baseline year population inputs'!$C$52</definedName>
+    <definedName name="diarrhoea_1_5mo">'Baseline year population inputs'!$C$52</definedName>
+    <definedName name="diarrhoea_12_23mo">'Baseline year population inputs'!$C$54</definedName>
+    <definedName name="diarrhoea_1mo">'Baseline year population inputs'!$C$51</definedName>
+    <definedName name="diarrhoea_24_59mo">'Baseline year population inputs'!$C$55</definedName>
+    <definedName name="diarrhoea_6_11mo">'Baseline year population inputs'!$C$53</definedName>
     <definedName name="end_year">'Baseline year population inputs'!$C$4</definedName>
-    <definedName name="famplan_unmet_need">'Baseline year population inputs'!$C$12</definedName>
-    <definedName name="food_insecure">'Baseline year population inputs'!$C$7</definedName>
-    <definedName name="frac_children_health_facility">'Baseline year population inputs'!$C$11</definedName>
-    <definedName name="frac_diarrhea_severe">'Baseline year population inputs'!$C$57</definedName>
-    <definedName name="frac_maize">'Baseline year population inputs'!$C$18</definedName>
-    <definedName name="frac_malaria_risk">'Baseline year population inputs'!$C$8</definedName>
+    <definedName name="famplan_unmet_need">'Baseline year population inputs'!$C$13</definedName>
+    <definedName name="food_insecure">'Baseline year population inputs'!$C$8</definedName>
+    <definedName name="frac_children_health_facility">'Baseline year population inputs'!$C$12</definedName>
+    <definedName name="frac_diarrhea_severe">'Baseline year population inputs'!$C$58</definedName>
+    <definedName name="frac_maize">'Baseline year population inputs'!$C$19</definedName>
+    <definedName name="frac_malaria_risk">'Baseline year population inputs'!$C$9</definedName>
     <definedName name="frac_mam_1_5months">'Nutritional status distribution'!$D$10</definedName>
     <definedName name="frac_mam_12_23months">'Nutritional status distribution'!$F$10</definedName>
     <definedName name="frac_mam_1month">'Nutritional status distribution'!$C$10</definedName>
     <definedName name="frac_mam_24_59months">'Nutritional status distribution'!$G$10</definedName>
     <definedName name="frac_mam_6_11months">'Nutritional status distribution'!$E$10</definedName>
     <definedName name="frac_MAMtoSAM">'Baseline year population inputs'!#REF!</definedName>
-    <definedName name="frac_other_staples">'Baseline year population inputs'!$C$19</definedName>
-    <definedName name="frac_PW_health_facility">'Baseline year population inputs'!$C$10</definedName>
-    <definedName name="frac_rice">'Baseline year population inputs'!$C$16</definedName>
+    <definedName name="frac_other_staples">'Baseline year population inputs'!$C$20</definedName>
+    <definedName name="frac_PW_health_facility">'Baseline year population inputs'!$C$11</definedName>
+    <definedName name="frac_rice">'Baseline year population inputs'!$C$17</definedName>
     <definedName name="frac_sam_1_5months">'Nutritional status distribution'!$D$11</definedName>
     <definedName name="frac_sam_12_23months">'Nutritional status distribution'!$F$11</definedName>
     <definedName name="frac_sam_1month">'Nutritional status distribution'!$C$11</definedName>
     <definedName name="frac_sam_24_59months">'Nutritional status distribution'!$G$11</definedName>
     <definedName name="frac_sam_6_11months">'Nutritional status distribution'!$E$11</definedName>
     <definedName name="frac_SAMtoMAM">'Baseline year population inputs'!#REF!</definedName>
-    <definedName name="frac_subsistence_farming">'Baseline year population inputs'!$C$15</definedName>
-    <definedName name="frac_wheat">'Baseline year population inputs'!$C$17</definedName>
-    <definedName name="infant_mortality">'Baseline year population inputs'!$C$37</definedName>
-    <definedName name="iron_deficiency_anaemia">'Baseline year population inputs'!$C$58</definedName>
+    <definedName name="frac_subsistence_farming">'Baseline year population inputs'!$C$16</definedName>
+    <definedName name="frac_wheat">'Baseline year population inputs'!$C$18</definedName>
+    <definedName name="infant_mortality">'Baseline year population inputs'!$C$38</definedName>
+    <definedName name="iron_deficiency_anaemia">'Baseline year population inputs'!$C$59</definedName>
     <definedName name="manage_mam">'Treatment of SAM'!$D$2</definedName>
-    <definedName name="maternal_mortality">'Baseline year population inputs'!$C$39</definedName>
-    <definedName name="neonatal_mortality">'Baseline year population inputs'!$C$36</definedName>
-    <definedName name="Percentage_of_pregnant_women_attending_health_facility">'Baseline year population inputs'!$C$10</definedName>
-    <definedName name="preterm_AGA">'Baseline year population inputs'!$C$45</definedName>
-    <definedName name="preterm_SGA">'Baseline year population inputs'!$C$44</definedName>
-    <definedName name="school_attendance">'Baseline year population inputs'!$C$9</definedName>
+    <definedName name="maternal_mortality">'Baseline year population inputs'!$C$40</definedName>
+    <definedName name="neonatal_mortality">'Baseline year population inputs'!$C$37</definedName>
+    <definedName name="Percentage_of_pregnant_women_attending_health_facility">'Baseline year population inputs'!$C$11</definedName>
+    <definedName name="preterm_AGA">'Baseline year population inputs'!$C$46</definedName>
+    <definedName name="preterm_SGA">'Baseline year population inputs'!$C$45</definedName>
+    <definedName name="school_attendance">'Baseline year population inputs'!$C$10</definedName>
     <definedName name="start_year">'Baseline year population inputs'!$C$3</definedName>
-    <definedName name="stillbirth" localSheetId="6">'Baseline year population inputs'!$C$38</definedName>
-    <definedName name="stillbirth">'Baseline year population inputs'!$C$41</definedName>
-    <definedName name="term_AGA">'Baseline year population inputs'!$C$47</definedName>
-    <definedName name="term_SGA">'Baseline year population inputs'!$C$46</definedName>
-    <definedName name="U5_mortality">'Baseline year population inputs'!$C$38</definedName>
+    <definedName name="stillbirth" localSheetId="6">'Baseline year population inputs'!$C$39</definedName>
+    <definedName name="stillbirth">'Baseline year population inputs'!$C$42</definedName>
+    <definedName name="term_AGA">'Baseline year population inputs'!$C$48</definedName>
+    <definedName name="term_SGA">'Baseline year population inputs'!$C$47</definedName>
+    <definedName name="U5_mortality">'Baseline year population inputs'!$C$39</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -163,7 +163,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -172,14 +172,51 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-The cost per child per year can be estimated as 
-= (cost per treatment episode) * (SAM prevalence) * 2.6
-Cost per treatment episode includes management of MAM (if selected) and is an average over delivery modalities. See user guide for further information</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The cost per child per year can be estimated as 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">= (cost per treatment episode) * (SAM prevalence) * 2.6
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Cost per treatment episode includes management of MAM (if selected) and is an average over delivery modalities. See user guide for further information</t>
         </r>
       </text>
     </comment>
@@ -315,7 +352,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="211">
   <si>
     <t>year</t>
   </si>
@@ -656,9 +693,6 @@
     <t>Number of births</t>
   </si>
   <si>
-    <t>Children under 5</t>
-  </si>
-  <si>
     <t>Total WRA</t>
   </si>
   <si>
@@ -948,6 +982,9 @@
   </si>
   <si>
     <t>IFAS for pregnant women (health facility)</t>
+  </si>
+  <si>
+    <t>Children under 5 population</t>
   </si>
 </sst>
 </file>
@@ -1956,7 +1993,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2133,6 +2170,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="727">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
@@ -4304,9 +4342,11 @@
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -4320,15 +4360,15 @@
         <v>100</v>
       </c>
       <c r="B1" s="59" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" s="59" t="s">
         <v>165</v>
-      </c>
-      <c r="C1" s="59" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B2" s="59"/>
       <c r="C2" s="59"/>
@@ -4336,7 +4376,7 @@
     <row r="3" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C3" s="87">
         <v>2017</v>
@@ -4345,7 +4385,7 @@
     <row r="4" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C4" s="88">
         <v>2030</v>
@@ -4362,82 +4402,82 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="19" t="s">
+        <v>210</v>
+      </c>
+      <c r="C7" s="90">
+        <v>9862402</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C8" s="24">
         <v>0.28199999999999997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="C8" s="23">
-        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B10" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C10" s="23">
         <v>0.23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="C10" s="24">
-        <v>0.51</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C11" s="24">
-        <v>0.37</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="24">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C13" s="24">
         <v>0.221</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="15"/>
-    </row>
     <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="15" t="s">
+      <c r="B14" s="15"/>
+    </row>
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="C15" s="23">
-        <v>0.3</v>
-      </c>
+      <c r="B15" s="22"/>
+      <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C16" s="23">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C17" s="23">
         <v>0.1</v>
@@ -4445,299 +4485,307 @@
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C18" s="23">
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="23">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="C19" s="26">
+      <c r="C20" s="26">
         <f>1-frac_rice-frac_wheat-frac_maize</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="15"/>
-    </row>
     <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="15" t="s">
+      <c r="B21" s="15"/>
+    </row>
+    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="15" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B22" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="C22" s="23">
-        <v>0.127</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C23" s="23">
-        <v>0.45200000000000001</v>
+        <v>0.127</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C24" s="23">
-        <v>0.33400000000000002</v>
+        <v>0.45200000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="23">
+        <v>0.33400000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B26" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="C25" s="23">
+      <c r="C26" s="23">
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-    </row>
     <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="15" t="s">
-        <v>198</v>
-      </c>
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
     </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B28" s="41" t="s">
-        <v>75</v>
-      </c>
-      <c r="C28" s="42">
-        <v>0.20799999999999999</v>
-      </c>
+    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C29" s="42">
-        <v>0.63700000000000001</v>
+        <v>0.20799999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C30" s="42">
-        <v>0.11899999999999999</v>
+        <v>0.63700000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="42">
+        <v>0.11899999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B32" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="C31" s="42">
+      <c r="C32" s="42">
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="B32" s="45" t="s">
-        <v>130</v>
-      </c>
-      <c r="C32" s="44">
-        <f>SUM(C28:C31)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
+    <row r="33" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="B33" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33" s="44">
+        <f>SUM(C29:C32)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="16"/>
-    </row>
-    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B36" s="60" t="s">
+      <c r="B36" s="9"/>
+      <c r="C36" s="16"/>
+    </row>
+    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B37" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="C36" s="25">
+      <c r="C37" s="25">
         <v>25</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B37" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="C37" s="25">
-        <v>43</v>
-      </c>
-      <c r="D37" s="20"/>
-      <c r="E37" s="21"/>
     </row>
     <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="19" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C38" s="25">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
+      <c r="E38" s="21"/>
     </row>
     <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="19" t="s">
-        <v>172</v>
+        <v>90</v>
       </c>
       <c r="C39" s="25">
-        <v>4.01</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
     </row>
     <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B40" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="C40" s="25">
+        <v>4.01</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B41" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="C40" s="23">
+      <c r="C41" s="23">
         <v>0.13</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B41" s="60" t="s">
+    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B42" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="C41" s="25">
+      <c r="C42" s="25">
         <v>22.4</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D42" s="20"/>
-    </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="15" t="s">
-        <v>134</v>
-      </c>
       <c r="D43" s="20"/>
     </row>
     <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B44" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C44" s="23">
-        <v>3.1E-2</v>
+      <c r="A44" s="15" t="s">
+        <v>133</v>
       </c>
       <c r="D44" s="20"/>
     </row>
     <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B45" s="19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C45" s="23">
-        <v>0.109</v>
+        <v>3.1E-2</v>
       </c>
       <c r="D45" s="20"/>
     </row>
     <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B46" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="23">
+        <v>0.109</v>
+      </c>
+      <c r="D46" s="20"/>
+    </row>
+    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B47" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C46" s="23">
+      <c r="C47" s="23">
         <v>0.36499999999999999</v>
       </c>
-      <c r="D46" s="20"/>
-      <c r="E46" s="21"/>
-    </row>
-    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B47" s="19" t="s">
+      <c r="D47" s="20"/>
+      <c r="E47" s="21"/>
+    </row>
+    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B48" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C47" s="26">
+      <c r="C48" s="26">
         <f>1-term_SGA-preterm_AGA-preterm_SGA</f>
         <v>0.495</v>
       </c>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-    </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
     </row>
     <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="15" t="s">
+      <c r="D49" s="20"/>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="D49" s="20"/>
-    </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B50" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="C50" s="7">
-        <v>1.66</v>
-      </c>
       <c r="D50" s="20"/>
     </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B51" s="19" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C51" s="7">
         <v>1.66</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D51" s="20"/>
+    </row>
+    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B52" s="19" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C52" s="7">
-        <v>5.64</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B53" s="19" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C53" s="7">
-        <v>5.43</v>
+        <v>5.64</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B54" s="19" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C54" s="7">
+        <v>5.43</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B55" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="C55" s="7">
         <v>1.91</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="15" t="s">
-        <v>135</v>
-      </c>
-    </row>
     <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B57" s="9" t="s">
+      <c r="A57" s="15" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B58" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C57" s="24">
+      <c r="C58" s="24">
         <v>0.2</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B58" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="C58" s="24">
+    <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B59" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C59" s="24">
         <v>0.42</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="4"/>
+    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4764,24 +4812,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="40" x14ac:dyDescent="0.2">
       <c r="A1" s="80" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B1" s="79" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C1" s="79" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D1" s="79" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E1" s="79" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="78" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B2" s="77" t="s">
         <v>32</v>
@@ -4897,15 +4945,15 @@
         <v>69</v>
       </c>
       <c r="B1" s="58" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C1" s="58" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B2" s="66" t="s">
         <v>59</v>
@@ -4914,7 +4962,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B3" s="66" t="s">
         <v>59</v>
@@ -4926,16 +4974,16 @@
         <v>58</v>
       </c>
       <c r="B4" s="66" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C4" s="66"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="70" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B5" s="66" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C5" s="66"/>
     </row>
@@ -4994,7 +5042,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" s="66" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
@@ -5076,7 +5124,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5106,23 +5154,23 @@
         <v>71</v>
       </c>
       <c r="B2" s="37">
-        <f>'Baseline year population inputs'!C50</f>
-        <v>1.66</v>
-      </c>
-      <c r="C2" s="37">
         <f>'Baseline year population inputs'!C51</f>
         <v>1.66</v>
       </c>
+      <c r="C2" s="37">
+        <f>'Baseline year population inputs'!C52</f>
+        <v>1.66</v>
+      </c>
       <c r="D2" s="37">
-        <f>'Baseline year population inputs'!C52</f>
+        <f>'Baseline year population inputs'!C53</f>
         <v>5.64</v>
       </c>
       <c r="E2" s="37">
-        <f>'Baseline year population inputs'!C53</f>
+        <f>'Baseline year population inputs'!C54</f>
         <v>5.43</v>
       </c>
       <c r="F2" s="37">
-        <f>'Baseline year population inputs'!C54</f>
+        <f>'Baseline year population inputs'!C55</f>
         <v>1.91</v>
       </c>
     </row>
@@ -5189,8 +5237,8 @@
   </sheetPr>
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5305,7 +5353,7 @@
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C3" s="51">
         <v>1</v>
@@ -5349,7 +5397,7 @@
     </row>
     <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C4" s="51">
         <v>1</v>
@@ -5393,7 +5441,7 @@
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C5" s="51">
         <v>0</v>
@@ -5439,7 +5487,7 @@
     </row>
     <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C6" s="51">
         <v>0</v>
@@ -5866,7 +5914,7 @@
     <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4"/>
       <c r="B16" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C16" s="52">
         <v>0</v>
@@ -5915,7 +5963,7 @@
     <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4"/>
       <c r="B17" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C17" s="52">
         <v>0</v>
@@ -6153,7 +6201,7 @@
         <v>37</v>
       </c>
       <c r="B23" s="84" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C23" s="52">
         <v>0</v>
@@ -6183,21 +6231,25 @@
         <v>0</v>
       </c>
       <c r="L23" s="51">
-        <v>1</v>
+        <f>famplan_unmet_need</f>
+        <v>0.221</v>
       </c>
       <c r="M23" s="51">
-        <v>1</v>
+        <f>famplan_unmet_need</f>
+        <v>0.221</v>
       </c>
       <c r="N23" s="51">
-        <v>1</v>
+        <f>famplan_unmet_need</f>
+        <v>0.221</v>
       </c>
       <c r="O23" s="51">
-        <v>1</v>
+        <f>famplan_unmet_need</f>
+        <v>0.221</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="84" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C24" s="52">
         <v>0</v>
@@ -6245,7 +6297,7 @@
     </row>
     <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="84" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C25" s="52">
         <v>0</v>
@@ -6293,7 +6345,7 @@
     </row>
     <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="84" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C26" s="52">
         <v>0</v>
@@ -6341,7 +6393,7 @@
     </row>
     <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="84" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C27" s="52">
         <v>0</v>
@@ -6906,22 +6958,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -6937,7 +6989,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6951,24 +7003,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="58" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B1" s="58" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C1" s="58" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D1" s="58" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E1" s="58" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="57" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="56">
         <v>0.9</v>
@@ -6986,7 +7038,7 @@
     </row>
     <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="57" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B3" s="56">
         <v>1</v>
@@ -7004,7 +7056,7 @@
     </row>
     <row r="4" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="57" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B4" s="56">
         <v>1</v>
@@ -7022,7 +7074,7 @@
     </row>
     <row r="5" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="57" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B5" s="56">
         <v>1</v>
@@ -7040,7 +7092,7 @@
     </row>
     <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="57" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B6" s="56">
         <v>1</v>
@@ -7058,7 +7110,7 @@
     </row>
     <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="57" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B7" s="56">
         <v>0.93</v>
@@ -7076,7 +7128,7 @@
     </row>
     <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="57" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B8" s="56">
         <v>0.5</v>
@@ -7094,7 +7146,7 @@
     </row>
     <row r="9" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="57" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B9" s="56">
         <v>0.5</v>
@@ -7112,7 +7164,7 @@
     </row>
     <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="57" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B10" s="56">
         <v>0.98</v>
@@ -7143,20 +7195,20 @@
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8.5" style="15" customWidth="1"/>
-    <col min="2" max="10" width="16.83203125" style="15" customWidth="1"/>
-    <col min="11" max="16384" width="14.5" style="15"/>
+    <col min="2" max="9" width="16.83203125" style="15" customWidth="1"/>
+    <col min="10" max="16384" width="14.5" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
@@ -7164,31 +7216,28 @@
         <v>112</v>
       </c>
       <c r="C1" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="31" t="s">
-        <v>52</v>
-      </c>
       <c r="H1" s="31" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="I1" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="J1" s="31" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="9">
         <f>start_year</f>
         <v>2017</v>
@@ -7197,34 +7246,31 @@
         <v>2110000</v>
       </c>
       <c r="C2" s="29">
-        <v>9862402</v>
+        <v>3032037</v>
       </c>
       <c r="D2" s="29">
-        <v>3032037</v>
+        <v>4756743</v>
       </c>
       <c r="E2" s="29">
-        <v>4756743</v>
+        <v>3406589</v>
       </c>
       <c r="F2" s="29">
-        <v>3406589</v>
-      </c>
-      <c r="G2" s="29">
         <v>2174712</v>
       </c>
+      <c r="G2" s="30">
+        <f t="shared" ref="G2:G40" si="0">C2+D2+E2+F2</f>
+        <v>13370081</v>
+      </c>
       <c r="H2" s="30">
-        <f t="shared" ref="H2:H40" si="0">D2+E2+F2+G2</f>
-        <v>13370081</v>
-      </c>
-      <c r="I2" s="30">
         <f>(B2 + stillbirth*B2/(1000-stillbirth))/(1-abortion)</f>
         <v>2480858.588708919</v>
       </c>
-      <c r="J2" s="30">
-        <f>H2-I2</f>
+      <c r="I2" s="30">
+        <f>G2-H2</f>
         <v>10889222.411291081</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9">
         <f t="shared" ref="A3:A40" si="1">IF($A$2+ROW(A3)-2&lt;=end_year,A2+1,"")</f>
         <v>2018</v>
@@ -7233,34 +7279,31 @@
         <v>2150000</v>
       </c>
       <c r="C3" s="29">
-        <v>10050371</v>
+        <v>3164674</v>
       </c>
       <c r="D3" s="29">
-        <v>3164674</v>
+        <v>4882700</v>
       </c>
       <c r="E3" s="29">
-        <v>4882700</v>
+        <v>3520083</v>
       </c>
       <c r="F3" s="29">
-        <v>3520083</v>
-      </c>
-      <c r="G3" s="29">
         <v>2275309</v>
       </c>
-      <c r="H3" s="30">
+      <c r="G3" s="30">
         <f t="shared" si="0"/>
         <v>13842766</v>
       </c>
+      <c r="H3" s="30">
+        <f>(B3 + stillbirth*B3/(1000-stillbirth))/(1-abortion)</f>
+        <v>2527889.0832815999</v>
+      </c>
       <c r="I3" s="30">
-        <f t="shared" ref="I3:I40" si="2">(B3 + stillbirth*B3/(1000-stillbirth))/(1-abortion)</f>
-        <v>2527889.0832815999</v>
-      </c>
-      <c r="J3" s="30">
-        <f t="shared" ref="J3:J15" si="3">H3-I3</f>
+        <f t="shared" ref="I3:I15" si="2">G3-H3</f>
         <v>11314876.916718401</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9">
         <f t="shared" si="1"/>
         <v>2019</v>
@@ -7269,34 +7312,31 @@
         <v>2200000</v>
       </c>
       <c r="C4" s="29">
-        <v>10237786</v>
+        <v>3296354</v>
       </c>
       <c r="D4" s="29">
-        <v>3296354</v>
+        <v>5018666</v>
       </c>
       <c r="E4" s="29">
-        <v>5018666</v>
+        <v>3634703</v>
       </c>
       <c r="F4" s="29">
-        <v>3634703</v>
-      </c>
-      <c r="G4" s="29">
         <v>2379017</v>
       </c>
-      <c r="H4" s="30">
+      <c r="G4" s="30">
         <f t="shared" si="0"/>
         <v>14328740</v>
       </c>
+      <c r="H4" s="30">
+        <f>(B4 + stillbirth*B4/(1000-stillbirth))/(1-abortion)</f>
+        <v>2586677.2014974509</v>
+      </c>
       <c r="I4" s="30">
         <f t="shared" si="2"/>
-        <v>2586677.2014974509</v>
-      </c>
-      <c r="J4" s="30">
-        <f t="shared" si="3"/>
         <v>11742062.79850255</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="9">
         <f t="shared" si="1"/>
         <v>2020</v>
@@ -7305,34 +7345,31 @@
         <v>2240000</v>
       </c>
       <c r="C5" s="29">
-        <v>10438537</v>
+        <v>3418969</v>
       </c>
       <c r="D5" s="29">
-        <v>3418969</v>
+        <v>5168014</v>
       </c>
       <c r="E5" s="29">
-        <v>5168014</v>
+        <v>3750324</v>
       </c>
       <c r="F5" s="29">
-        <v>3750324</v>
-      </c>
-      <c r="G5" s="29">
         <v>2484409</v>
       </c>
-      <c r="H5" s="30">
+      <c r="G5" s="30">
         <f t="shared" si="0"/>
         <v>14821716</v>
       </c>
+      <c r="H5" s="30">
+        <f>(B5 + stillbirth*B5/(1000-stillbirth))/(1-abortion)</f>
+        <v>2633707.6960701318</v>
+      </c>
       <c r="I5" s="30">
         <f t="shared" si="2"/>
-        <v>2633707.6960701318</v>
-      </c>
-      <c r="J5" s="30">
-        <f t="shared" si="3"/>
         <v>12188008.303929869</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="9">
         <f t="shared" si="1"/>
         <v>2021</v>
@@ -7341,34 +7378,31 @@
         <v>2280000</v>
       </c>
       <c r="C6" s="29">
-        <v>10636534</v>
+        <v>3532758</v>
       </c>
       <c r="D6" s="29">
-        <v>3532758</v>
+        <v>5332455</v>
       </c>
       <c r="E6" s="29">
-        <v>5332455</v>
+        <v>3869436</v>
       </c>
       <c r="F6" s="29">
-        <v>3869436</v>
-      </c>
-      <c r="G6" s="29">
         <v>2592003</v>
       </c>
-      <c r="H6" s="30">
+      <c r="G6" s="30">
         <f t="shared" si="0"/>
         <v>15326652</v>
       </c>
+      <c r="H6" s="30">
+        <f>(B6 + stillbirth*B6/(1000-stillbirth))/(1-abortion)</f>
+        <v>2680738.1906428128</v>
+      </c>
       <c r="I6" s="30">
         <f t="shared" si="2"/>
-        <v>2680738.1906428128</v>
-      </c>
-      <c r="J6" s="30">
-        <f t="shared" si="3"/>
         <v>12645913.809357187</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="9">
         <f t="shared" si="1"/>
         <v>2022</v>
@@ -7377,34 +7411,31 @@
         <v>2330000</v>
       </c>
       <c r="C7" s="29">
-        <v>10854967</v>
+        <v>3637390</v>
       </c>
       <c r="D7" s="29">
-        <v>3637390</v>
+        <v>5508952</v>
       </c>
       <c r="E7" s="29">
-        <v>5508952</v>
+        <v>3990560</v>
       </c>
       <c r="F7" s="29">
-        <v>3990560</v>
-      </c>
-      <c r="G7" s="29">
         <v>2701259</v>
       </c>
-      <c r="H7" s="30">
+      <c r="G7" s="30">
         <f t="shared" si="0"/>
         <v>15838161</v>
       </c>
+      <c r="H7" s="30">
+        <f>(B7 + stillbirth*B7/(1000-stillbirth))/(1-abortion)</f>
+        <v>2739526.3088586638</v>
+      </c>
       <c r="I7" s="30">
         <f t="shared" si="2"/>
-        <v>2739526.3088586638</v>
-      </c>
-      <c r="J7" s="30">
-        <f t="shared" si="3"/>
         <v>13098634.691141337</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="9">
         <f t="shared" si="1"/>
         <v>2023</v>
@@ -7413,34 +7444,31 @@
         <v>2380000</v>
       </c>
       <c r="C8" s="29">
-        <v>11089897</v>
+        <v>3737403</v>
       </c>
       <c r="D8" s="29">
-        <v>3737403</v>
+        <v>5696990</v>
       </c>
       <c r="E8" s="29">
-        <v>5696990</v>
+        <v>4112898</v>
       </c>
       <c r="F8" s="29">
-        <v>4112898</v>
-      </c>
-      <c r="G8" s="29">
         <v>2811667</v>
       </c>
-      <c r="H8" s="30">
+      <c r="G8" s="30">
         <f t="shared" si="0"/>
         <v>16358958</v>
       </c>
+      <c r="H8" s="30">
+        <f>(B8 + stillbirth*B8/(1000-stillbirth))/(1-abortion)</f>
+        <v>2798314.4270745148</v>
+      </c>
       <c r="I8" s="30">
         <f t="shared" si="2"/>
-        <v>2798314.4270745148</v>
-      </c>
-      <c r="J8" s="30">
-        <f t="shared" si="3"/>
         <v>13560643.572925486</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9">
         <f t="shared" si="1"/>
         <v>2024</v>
@@ -7449,34 +7477,31 @@
         <v>2420000</v>
       </c>
       <c r="C9" s="29">
-        <v>11331595</v>
+        <v>3840674</v>
       </c>
       <c r="D9" s="29">
-        <v>3840674</v>
+        <v>5895615</v>
       </c>
       <c r="E9" s="29">
-        <v>5895615</v>
+        <v>4235117</v>
       </c>
       <c r="F9" s="29">
-        <v>4235117</v>
-      </c>
-      <c r="G9" s="29">
         <v>2922818</v>
       </c>
-      <c r="H9" s="30">
+      <c r="G9" s="30">
         <f t="shared" si="0"/>
         <v>16894224</v>
       </c>
+      <c r="H9" s="30">
+        <f>(B9 + stillbirth*B9/(1000-stillbirth))/(1-abortion)</f>
+        <v>2845344.9216471957</v>
+      </c>
       <c r="I9" s="30">
         <f t="shared" si="2"/>
-        <v>2845344.9216471957</v>
-      </c>
-      <c r="J9" s="30">
-        <f t="shared" si="3"/>
         <v>14048879.078352805</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="9">
         <f t="shared" si="1"/>
         <v>2025</v>
@@ -7485,34 +7510,31 @@
         <v>2480000</v>
       </c>
       <c r="C10" s="29">
-        <v>11574198</v>
+        <v>3951644</v>
       </c>
       <c r="D10" s="29">
-        <v>3951644</v>
+        <v>6103745</v>
       </c>
       <c r="E10" s="29">
-        <v>6103745</v>
+        <v>4356516</v>
       </c>
       <c r="F10" s="29">
-        <v>4356516</v>
-      </c>
-      <c r="G10" s="29">
         <v>3034340</v>
       </c>
-      <c r="H10" s="30">
+      <c r="G10" s="30">
         <f t="shared" si="0"/>
         <v>17446245</v>
       </c>
+      <c r="H10" s="30">
+        <f>(B10 + stillbirth*B10/(1000-stillbirth))/(1-abortion)</f>
+        <v>2915890.6635062173</v>
+      </c>
       <c r="I10" s="30">
         <f t="shared" si="2"/>
-        <v>2915890.6635062173</v>
-      </c>
-      <c r="J10" s="30">
-        <f t="shared" si="3"/>
         <v>14530354.336493783</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="9">
         <f t="shared" si="1"/>
         <v>2026</v>
@@ -7521,34 +7543,31 @@
         <v>2530000</v>
       </c>
       <c r="C11" s="29">
-        <v>11838769</v>
+        <v>4065313</v>
       </c>
       <c r="D11" s="29">
-        <v>4065313</v>
+        <v>6319831</v>
       </c>
       <c r="E11" s="29">
-        <v>6319831</v>
+        <v>4477188</v>
       </c>
       <c r="F11" s="29">
-        <v>4477188</v>
-      </c>
-      <c r="G11" s="29">
         <v>3144612</v>
       </c>
-      <c r="H11" s="30">
+      <c r="G11" s="30">
         <f t="shared" si="0"/>
         <v>18006944</v>
       </c>
+      <c r="H11" s="30">
+        <f>(B11 + stillbirth*B11/(1000-stillbirth))/(1-abortion)</f>
+        <v>2974678.7817220683</v>
+      </c>
       <c r="I11" s="30">
         <f t="shared" si="2"/>
-        <v>2974678.7817220683</v>
-      </c>
-      <c r="J11" s="30">
-        <f t="shared" si="3"/>
         <v>15032265.218277931</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9">
         <f t="shared" si="1"/>
         <v>2027</v>
@@ -7557,34 +7576,31 @@
         <v>2580000</v>
       </c>
       <c r="C12" s="29">
-        <v>12092177</v>
+        <v>4185562</v>
       </c>
       <c r="D12" s="29">
-        <v>4185562</v>
+        <v>6545116</v>
       </c>
       <c r="E12" s="29">
-        <v>6545116</v>
+        <v>4597739</v>
       </c>
       <c r="F12" s="29">
-        <v>4597739</v>
-      </c>
-      <c r="G12" s="29">
         <v>3255252</v>
       </c>
-      <c r="H12" s="30">
+      <c r="G12" s="30">
         <f t="shared" si="0"/>
         <v>18583669</v>
       </c>
+      <c r="H12" s="30">
+        <f>(B12 + stillbirth*B12/(1000-stillbirth))/(1-abortion)</f>
+        <v>3033466.8999379198</v>
+      </c>
       <c r="I12" s="30">
         <f t="shared" si="2"/>
-        <v>3033466.8999379198</v>
-      </c>
-      <c r="J12" s="30">
-        <f t="shared" si="3"/>
         <v>15550202.10006208</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9">
         <f t="shared" si="1"/>
         <v>2028</v>
@@ -7593,34 +7609,31 @@
         <v>2630000</v>
       </c>
       <c r="C13" s="29">
-        <v>12338218</v>
+        <v>4309237</v>
       </c>
       <c r="D13" s="29">
-        <v>4309237</v>
+        <v>6776307</v>
       </c>
       <c r="E13" s="29">
-        <v>6776307</v>
+        <v>4722286</v>
       </c>
       <c r="F13" s="29">
-        <v>4722286</v>
-      </c>
-      <c r="G13" s="29">
         <v>3366750</v>
       </c>
-      <c r="H13" s="30">
+      <c r="G13" s="30">
         <f t="shared" si="0"/>
         <v>19174580</v>
       </c>
+      <c r="H13" s="30">
+        <f>(B13 + stillbirth*B13/(1000-stillbirth))/(1-abortion)</f>
+        <v>3092255.0181537713</v>
+      </c>
       <c r="I13" s="30">
         <f t="shared" si="2"/>
-        <v>3092255.0181537713</v>
-      </c>
-      <c r="J13" s="30">
-        <f t="shared" si="3"/>
         <v>16082324.981846228</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9">
         <f t="shared" si="1"/>
         <v>2029</v>
@@ -7629,34 +7642,31 @@
         <v>2690000</v>
       </c>
       <c r="C14" s="29">
-        <v>12584924</v>
+        <v>4430738</v>
       </c>
       <c r="D14" s="29">
-        <v>4430738</v>
+        <v>7008703</v>
       </c>
       <c r="E14" s="29">
-        <v>7008703</v>
+        <v>4856898</v>
       </c>
       <c r="F14" s="29">
-        <v>4856898</v>
-      </c>
-      <c r="G14" s="29">
         <v>3479917</v>
       </c>
-      <c r="H14" s="30">
+      <c r="G14" s="30">
         <f t="shared" si="0"/>
         <v>19776256</v>
       </c>
+      <c r="H14" s="30">
+        <f>(B14 + stillbirth*B14/(1000-stillbirth))/(1-abortion)</f>
+        <v>3162800.7600127924</v>
+      </c>
       <c r="I14" s="30">
         <f t="shared" si="2"/>
-        <v>3162800.7600127924</v>
-      </c>
-      <c r="J14" s="30">
-        <f t="shared" si="3"/>
         <v>16613455.239987208</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9">
         <f t="shared" si="1"/>
         <v>2030</v>
@@ -7665,34 +7675,31 @@
         <v>2740000</v>
       </c>
       <c r="C15" s="29">
-        <v>12839335</v>
+        <v>4546624</v>
       </c>
       <c r="D15" s="29">
-        <v>4546624</v>
+        <v>7239465</v>
       </c>
       <c r="E15" s="29">
-        <v>7239465</v>
+        <v>5005361</v>
       </c>
       <c r="F15" s="29">
-        <v>5005361</v>
-      </c>
-      <c r="G15" s="29">
         <v>3595278</v>
       </c>
-      <c r="H15" s="30">
+      <c r="G15" s="30">
         <f t="shared" si="0"/>
         <v>20386728</v>
       </c>
+      <c r="H15" s="30">
+        <f>(B15 + stillbirth*B15/(1000-stillbirth))/(1-abortion)</f>
+        <v>3221588.8782286434</v>
+      </c>
       <c r="I15" s="30">
         <f t="shared" si="2"/>
-        <v>3221588.8782286434</v>
-      </c>
-      <c r="J15" s="30">
-        <f t="shared" si="3"/>
         <v>17165139.121771358</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7702,21 +7709,20 @@
       <c r="D16" s="29"/>
       <c r="E16" s="29"/>
       <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
+      <c r="G16" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H16" s="30">
-        <f t="shared" si="0"/>
+        <f>(B16 + stillbirth*B16/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I16" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="30">
-        <f t="shared" ref="J16:J40" si="4">H16-I16</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" ref="I16:I40" si="3">G16-H16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7726,21 +7732,20 @@
       <c r="D17" s="29"/>
       <c r="E17" s="29"/>
       <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
+      <c r="G17" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H17" s="30">
-        <f t="shared" si="0"/>
+        <f>(B17 + stillbirth*B17/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I17" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7750,21 +7755,20 @@
       <c r="D18" s="29"/>
       <c r="E18" s="29"/>
       <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
+      <c r="G18" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H18" s="30">
-        <f t="shared" si="0"/>
+        <f>(B18 + stillbirth*B18/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I18" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7774,21 +7778,20 @@
       <c r="D19" s="29"/>
       <c r="E19" s="29"/>
       <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
+      <c r="G19" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H19" s="30">
-        <f t="shared" si="0"/>
+        <f>(B19 + stillbirth*B19/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I19" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J19" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7798,21 +7801,20 @@
       <c r="D20" s="29"/>
       <c r="E20" s="29"/>
       <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
+      <c r="G20" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H20" s="30">
-        <f t="shared" si="0"/>
+        <f>(B20 + stillbirth*B20/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I20" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J20" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7822,21 +7824,20 @@
       <c r="D21" s="29"/>
       <c r="E21" s="29"/>
       <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
+      <c r="G21" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H21" s="30">
-        <f t="shared" si="0"/>
+        <f>(B21 + stillbirth*B21/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I21" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J21" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7846,21 +7847,20 @@
       <c r="D22" s="29"/>
       <c r="E22" s="29"/>
       <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
+      <c r="G22" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H22" s="30">
-        <f t="shared" si="0"/>
+        <f>(B22 + stillbirth*B22/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I22" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J22" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7870,21 +7870,20 @@
       <c r="D23" s="29"/>
       <c r="E23" s="29"/>
       <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
+      <c r="G23" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H23" s="30">
-        <f t="shared" si="0"/>
+        <f>(B23 + stillbirth*B23/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I23" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J23" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7894,21 +7893,20 @@
       <c r="D24" s="29"/>
       <c r="E24" s="29"/>
       <c r="F24" s="29"/>
-      <c r="G24" s="29"/>
+      <c r="G24" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H24" s="30">
-        <f t="shared" si="0"/>
+        <f>(B24 + stillbirth*B24/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I24" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J24" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7918,21 +7916,20 @@
       <c r="D25" s="29"/>
       <c r="E25" s="29"/>
       <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
+      <c r="G25" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H25" s="30">
-        <f t="shared" si="0"/>
+        <f>(B25 + stillbirth*B25/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I25" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J25" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7942,21 +7939,20 @@
       <c r="D26" s="29"/>
       <c r="E26" s="29"/>
       <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
+      <c r="G26" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H26" s="30">
-        <f t="shared" si="0"/>
+        <f>(B26 + stillbirth*B26/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I26" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J26" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7966,21 +7962,20 @@
       <c r="D27" s="29"/>
       <c r="E27" s="29"/>
       <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
+      <c r="G27" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H27" s="30">
-        <f t="shared" si="0"/>
+        <f>(B27 + stillbirth*B27/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I27" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J27" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -7990,21 +7985,20 @@
       <c r="D28" s="29"/>
       <c r="E28" s="29"/>
       <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
+      <c r="G28" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H28" s="30">
-        <f t="shared" si="0"/>
+        <f>(B28 + stillbirth*B28/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I28" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J28" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8014,21 +8008,20 @@
       <c r="D29" s="29"/>
       <c r="E29" s="29"/>
       <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
+      <c r="G29" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H29" s="30">
-        <f t="shared" si="0"/>
+        <f>(B29 + stillbirth*B29/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I29" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J29" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8038,21 +8031,20 @@
       <c r="D30" s="29"/>
       <c r="E30" s="29"/>
       <c r="F30" s="29"/>
-      <c r="G30" s="29"/>
+      <c r="G30" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H30" s="30">
-        <f t="shared" si="0"/>
+        <f>(B30 + stillbirth*B30/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I30" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J30" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8062,21 +8054,20 @@
       <c r="D31" s="29"/>
       <c r="E31" s="29"/>
       <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
+      <c r="G31" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H31" s="30">
-        <f t="shared" si="0"/>
+        <f>(B31 + stillbirth*B31/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I31" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J31" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8086,21 +8077,20 @@
       <c r="D32" s="29"/>
       <c r="E32" s="29"/>
       <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
+      <c r="G32" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H32" s="30">
-        <f t="shared" si="0"/>
+        <f>(B32 + stillbirth*B32/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I32" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J32" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8110,21 +8100,20 @@
       <c r="D33" s="29"/>
       <c r="E33" s="29"/>
       <c r="F33" s="29"/>
-      <c r="G33" s="29"/>
+      <c r="G33" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H33" s="30">
-        <f t="shared" si="0"/>
+        <f>(B33 + stillbirth*B33/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I33" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J33" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8134,21 +8123,20 @@
       <c r="D34" s="29"/>
       <c r="E34" s="29"/>
       <c r="F34" s="29"/>
-      <c r="G34" s="29"/>
+      <c r="G34" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H34" s="30">
-        <f t="shared" si="0"/>
+        <f>(B34 + stillbirth*B34/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I34" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J34" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8158,21 +8146,20 @@
       <c r="D35" s="29"/>
       <c r="E35" s="29"/>
       <c r="F35" s="29"/>
-      <c r="G35" s="29"/>
+      <c r="G35" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H35" s="30">
-        <f t="shared" si="0"/>
+        <f>(B35 + stillbirth*B35/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I35" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J35" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8182,21 +8169,20 @@
       <c r="D36" s="29"/>
       <c r="E36" s="29"/>
       <c r="F36" s="29"/>
-      <c r="G36" s="29"/>
+      <c r="G36" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H36" s="30">
-        <f t="shared" si="0"/>
+        <f>(B36 + stillbirth*B36/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I36" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J36" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8206,21 +8192,20 @@
       <c r="D37" s="29"/>
       <c r="E37" s="29"/>
       <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
+      <c r="G37" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H37" s="30">
-        <f t="shared" si="0"/>
+        <f>(B37 + stillbirth*B37/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I37" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J37" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8230,21 +8215,20 @@
       <c r="D38" s="29"/>
       <c r="E38" s="29"/>
       <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
+      <c r="G38" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H38" s="30">
-        <f t="shared" si="0"/>
+        <f>(B38 + stillbirth*B38/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I38" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J38" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8254,21 +8238,20 @@
       <c r="D39" s="29"/>
       <c r="E39" s="29"/>
       <c r="F39" s="29"/>
-      <c r="G39" s="29"/>
+      <c r="G39" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H39" s="30">
-        <f t="shared" si="0"/>
+        <f>(B39 + stillbirth*B39/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I39" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J39" s="30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -8278,22 +8261,21 @@
       <c r="D40" s="29"/>
       <c r="E40" s="29"/>
       <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
+      <c r="G40" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H40" s="30">
-        <f t="shared" si="0"/>
+        <f>(B40 + stillbirth*B40/(1000-stillbirth))/(1-abortion)</f>
         <v>0</v>
       </c>
       <c r="I40" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J40" s="30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:J40">
+  <conditionalFormatting sqref="B2:I40">
     <cfRule type="expression" dxfId="0" priority="9">
       <formula>$A2=""</formula>
     </cfRule>
@@ -8311,7 +8293,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8957,7 +8939,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8992,10 +8974,10 @@
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C2" s="46">
         <f>IFERROR(1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE), "")</f>
@@ -9021,7 +9003,7 @@
     <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5"/>
       <c r="B3" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C3" s="46">
         <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE) - SUM(C4:C5), "")</f>
@@ -9047,7 +9029,7 @@
     <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5"/>
       <c r="B4" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C4" s="39">
         <v>8.7000000000000008E-2</v>
@@ -9068,7 +9050,7 @@
     <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5"/>
       <c r="B5" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C5" s="39">
         <v>4.5999999999999999E-2</v>
@@ -9104,10 +9086,10 @@
     </row>
     <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C8" s="46">
         <f>IFERROR(1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE), "")</f>
@@ -9132,7 +9114,7 @@
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C9" s="46">
         <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE) - SUM(C10:C11), "")</f>
@@ -9157,7 +9139,7 @@
     </row>
     <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C10" s="39">
         <v>5.3999999999999999E-2</v>
@@ -9177,7 +9159,7 @@
     </row>
     <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C11" s="39">
         <v>0.04</v>
@@ -9255,7 +9237,7 @@
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C14" s="47">
         <v>0.1</v>
@@ -9421,7 +9403,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="61" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C2" s="39">
         <v>0.84</v>
@@ -9441,7 +9423,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B3" s="61" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C3" s="39">
         <v>9.1999999999999998E-2</v>
@@ -9461,7 +9443,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B4" s="61" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C4" s="39">
         <v>5.8000000000000003E-2</v>
@@ -9481,7 +9463,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B5" s="61" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C5" s="46">
         <f>1-SUM(C2:C4)</f>
@@ -9528,10 +9510,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C1">
         <v>2010</v>
@@ -9563,10 +9545,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C2" s="39"/>
       <c r="D2" s="39"/>
@@ -9583,10 +9565,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
@@ -9603,10 +9585,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C6" s="39"/>
       <c r="D6" s="39"/>
@@ -9634,7 +9616,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B8" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C8" s="39"/>
       <c r="D8" s="39"/>
@@ -9648,10 +9630,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
@@ -9665,7 +9647,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B11" s="50" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C11" s="39"/>
       <c r="D11" s="39"/>
@@ -9682,7 +9664,7 @@
         <v>74</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C13" s="39"/>
       <c r="D13" s="39"/>
@@ -9696,7 +9678,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B14" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C14" s="39"/>
       <c r="D14" s="39"/>
@@ -9722,7 +9704,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9735,24 +9717,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="68" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B1" s="69" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C1" s="69" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D1" s="69" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E1" s="69" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="67" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B2" s="64" t="s">
         <v>32</v>
@@ -9769,8 +9751,8 @@
       <c r="B3" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="66" t="s">
-        <v>195</v>
+      <c r="C3" s="66" t="b">
+        <v>1</v>
       </c>
       <c r="D3" s="66"/>
       <c r="E3" s="81" t="str">
@@ -9783,8 +9765,8 @@
       <c r="B4" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="66" t="s">
-        <v>195</v>
+      <c r="C4" s="66" t="b">
+        <v>1</v>
       </c>
       <c r="D4" s="66"/>
       <c r="E4" s="81" t="str">
@@ -9797,8 +9779,8 @@
       <c r="B5" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="66" t="s">
-        <v>195</v>
+      <c r="C5" s="66" t="b">
+        <v>1</v>
       </c>
       <c r="D5" s="66"/>
       <c r="E5" s="81" t="str">
@@ -9811,8 +9793,8 @@
       <c r="B6" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="66" t="s">
-        <v>195</v>
+      <c r="C6" s="66" t="b">
+        <v>1</v>
       </c>
       <c r="D6" s="66"/>
       <c r="E6" s="81" t="str">
@@ -9823,7 +9805,7 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="65"/>
       <c r="B7" s="64" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C7" s="63"/>
       <c r="D7" s="62"/>
@@ -9831,14 +9813,14 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="67" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B9" s="64" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="66"/>
-      <c r="D9" s="66" t="s">
-        <v>195</v>
+      <c r="D9" s="66" t="b">
+        <v>0</v>
       </c>
       <c r="E9" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
@@ -9896,7 +9878,7 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" s="65"/>
       <c r="B14" s="64" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C14" s="63"/>
       <c r="D14" s="62"/>
@@ -9904,14 +9886,14 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="67" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B16" s="64" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="66"/>
       <c r="D16" s="66" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E16" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
@@ -9925,7 +9907,7 @@
       </c>
       <c r="C17" s="66"/>
       <c r="D17" s="66" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E17" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
@@ -9939,7 +9921,7 @@
       </c>
       <c r="C18" s="66"/>
       <c r="D18" s="66" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E18" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
@@ -9953,7 +9935,7 @@
       </c>
       <c r="C19" s="66"/>
       <c r="D19" s="66" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E19" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
@@ -9967,7 +9949,7 @@
       </c>
       <c r="C20" s="66"/>
       <c r="D20" s="66" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E20" s="81" t="str">
         <f>IF(E$7="","",E$7)</f>
@@ -9977,7 +9959,7 @@
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="65"/>
       <c r="B21" s="64" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C21" s="63"/>
       <c r="D21" s="62"/>
@@ -10010,16 +9992,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="85" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B1" s="69" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="86" t="s">
         <v>182</v>
       </c>
-      <c r="C1" s="86" t="s">
-        <v>183</v>
-      </c>
       <c r="D1" s="86" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -10030,19 +10012,19 @@
         <v>67</v>
       </c>
       <c r="C2" s="64" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D2" s="66"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="86" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B3" s="64" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C3" s="64" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D3" s="66"/>
     </row>
@@ -10081,13 +10063,13 @@
         <v>Baseline (2017) coverage</v>
       </c>
       <c r="C1" s="73" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D1" s="73" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E1" s="73" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10104,7 +10086,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10121,7 +10103,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10138,12 +10120,12 @@
         <v>90</v>
       </c>
       <c r="E4" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="70" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B5" s="71">
         <v>0</v>
@@ -10155,12 +10137,12 @@
         <v>1</v>
       </c>
       <c r="E5" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="70" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B6" s="71">
         <v>0</v>
@@ -10172,7 +10154,7 @@
         <v>0.82</v>
       </c>
       <c r="E6" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10189,7 +10171,7 @@
         <v>0.25</v>
       </c>
       <c r="E7" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10206,7 +10188,7 @@
         <v>0.75</v>
       </c>
       <c r="E8" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10223,12 +10205,12 @@
         <v>0.19</v>
       </c>
       <c r="E9" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="84" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B10" s="71">
         <v>0</v>
@@ -10240,12 +10222,12 @@
         <v>0.73</v>
       </c>
       <c r="E10" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="84" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B11" s="71">
         <v>0</v>
@@ -10257,12 +10239,12 @@
         <v>1.78</v>
       </c>
       <c r="E11" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="84" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B12" s="71">
         <v>0</v>
@@ -10274,12 +10256,12 @@
         <v>0.24</v>
       </c>
       <c r="E12" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="84" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B13" s="71">
         <v>0</v>
@@ -10291,12 +10273,12 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="E13" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B14" s="71">
         <v>0</v>
@@ -10308,12 +10290,12 @@
         <v>0.73</v>
       </c>
       <c r="E14" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B15" s="71">
         <v>0</v>
@@ -10325,7 +10307,7 @@
         <v>1.78</v>
       </c>
       <c r="E15" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10342,7 +10324,7 @@
         <v>2.06</v>
       </c>
       <c r="E16" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10359,12 +10341,12 @@
         <v>0.05</v>
       </c>
       <c r="E17" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="70" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B18" s="71">
         <v>0</v>
@@ -10377,12 +10359,12 @@
         <v>3.66</v>
       </c>
       <c r="E18" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="70" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B19" s="71">
         <v>0</v>
@@ -10395,12 +10377,12 @@
         <v>3.78</v>
       </c>
       <c r="E19" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="70" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B20" s="71">
         <v>0</v>
@@ -10413,12 +10395,12 @@
         <v>14.270000000000001</v>
       </c>
       <c r="E20" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="70" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B21" s="71">
         <v>0</v>
@@ -10430,12 +10412,12 @@
         <v>8.84</v>
       </c>
       <c r="E21" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="70" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B22" s="71">
         <v>0</v>
@@ -10447,7 +10429,7 @@
         <v>50</v>
       </c>
       <c r="E22" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10464,7 +10446,7 @@
         <v>2.61</v>
       </c>
       <c r="E23" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10481,7 +10463,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10498,12 +10480,12 @@
         <v>1</v>
       </c>
       <c r="E25" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="70" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B26" s="71">
         <v>0.1</v>
@@ -10515,7 +10497,7 @@
         <v>4.6500000000000004</v>
       </c>
       <c r="E26" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10532,7 +10514,7 @@
         <v>3.78</v>
       </c>
       <c r="E27" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10549,7 +10531,7 @@
         <v>1</v>
       </c>
       <c r="E28" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10566,7 +10548,7 @@
         <v>48</v>
       </c>
       <c r="E29" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10583,7 +10565,7 @@
         <v>5.3</v>
       </c>
       <c r="E30" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10600,7 +10582,7 @@
         <v>0.41</v>
       </c>
       <c r="E31" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10617,7 +10599,7 @@
         <v>0.9</v>
       </c>
       <c r="E32" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10634,7 +10616,7 @@
         <v>0.9</v>
       </c>
       <c r="E33" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10651,7 +10633,7 @@
         <v>79</v>
       </c>
       <c r="E34" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10668,7 +10650,7 @@
         <v>31</v>
       </c>
       <c r="E35" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10685,7 +10667,7 @@
         <v>102</v>
       </c>
       <c r="E36" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F36" s="53"/>
     </row>
@@ -10703,7 +10685,7 @@
         <v>5.53</v>
       </c>
       <c r="E37" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10720,7 +10702,7 @@
         <v>1</v>
       </c>
       <c r="E38" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>